<commit_message>
added desired hp to fuel simple chart
Signed-off-by: akudlacek <7029639+akudlacek@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/gear_hp_mileage_calc.xlsx
+++ b/gear_hp_mileage_calc.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GD\EFILive\Tuning Calc\cummins_tuning_calc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16005"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16005" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Gear" sheetId="12" r:id="rId1"/>
@@ -59,7 +64,7 @@
     <definedName name="TransferCase" localSheetId="3">'Reference Ratio Table'!$27:$27</definedName>
     <definedName name="Wheel_Diameter">Gear!$B$16</definedName>
   </definedNames>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -74,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="150">
   <si>
     <t>HP</t>
   </si>
@@ -586,16 +591,19 @@
       <t>17</t>
     </r>
   </si>
+  <si>
+    <t>DESIRED HP (user input)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -732,7 +740,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -1031,6 +1039,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1040,7 +1063,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="188">
+  <cellXfs count="195">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1480,8 +1503,14 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1489,16 +1518,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1509,14 +1535,8 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1533,11 +1553,29 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1855,14 +1893,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.140625" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" customWidth="1"/>
@@ -1876,7 +1914,7 @@
     <col min="28" max="28" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="131" t="s">
         <v>147</v>
       </c>
@@ -1910,7 +1948,7 @@
       <c r="AA1" s="144"/>
       <c r="AB1" s="145"/>
     </row>
-    <row r="2" spans="1:29" ht="15.75" thickBot="1">
+    <row r="2" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="133"/>
       <c r="B2" s="134"/>
       <c r="D2" s="139"/>
@@ -1942,7 +1980,7 @@
       <c r="AA2" s="6"/>
       <c r="AB2" s="7"/>
     </row>
-    <row r="3" spans="1:29" ht="15.75" thickBot="1">
+    <row r="3" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="133"/>
       <c r="B3" s="134"/>
       <c r="D3" s="139"/>
@@ -1975,7 +2013,7 @@
       <c r="AB3" s="9"/>
       <c r="AC3" s="11"/>
     </row>
-    <row r="4" spans="1:29" ht="15.75" thickBot="1">
+    <row r="4" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="133"/>
       <c r="B4" s="134"/>
       <c r="D4" s="141"/>
@@ -2040,7 +2078,7 @@
       <c r="AB4" s="9"/>
       <c r="AC4" s="11"/>
     </row>
-    <row r="5" spans="1:29" ht="15.75" thickBot="1">
+    <row r="5" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="133"/>
       <c r="B5" s="134"/>
       <c r="D5" s="13" t="s">
@@ -2128,7 +2166,7 @@
       <c r="AB5" s="9"/>
       <c r="AC5" s="11"/>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="133"/>
       <c r="B6" s="134"/>
       <c r="D6" s="11" t="s">
@@ -2198,7 +2236,7 @@
       <c r="AB6" s="9"/>
       <c r="AC6" s="11"/>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="133"/>
       <c r="B7" s="134"/>
       <c r="D7" s="11" t="s">
@@ -2294,7 +2332,7 @@
       </c>
       <c r="AC7" s="11"/>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="133"/>
       <c r="B8" s="134"/>
       <c r="D8" s="11" t="s">
@@ -2385,7 +2423,7 @@
       </c>
       <c r="AB8" s="157"/>
     </row>
-    <row r="9" spans="1:29" ht="15.75" thickBot="1">
+    <row r="9" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="135"/>
       <c r="B9" s="136"/>
       <c r="D9" s="21" t="s">
@@ -2476,7 +2514,7 @@
       </c>
       <c r="AB9" s="157"/>
     </row>
-    <row r="10" spans="1:29">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="159" t="s">
         <v>34</v>
       </c>
@@ -2564,7 +2602,7 @@
       </c>
       <c r="AB10" s="157"/>
     </row>
-    <row r="11" spans="1:29">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="161" t="s">
         <v>37</v>
       </c>
@@ -2652,7 +2690,7 @@
       </c>
       <c r="AB11" s="157"/>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="D12" s="1"/>
@@ -2738,7 +2776,7 @@
       </c>
       <c r="AB12" s="157"/>
     </row>
-    <row r="13" spans="1:29" ht="15.75" thickBot="1">
+    <row r="13" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="163" t="s">
         <v>148</v>
       </c>
@@ -2824,7 +2862,7 @@
       </c>
       <c r="AB13" s="157"/>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>41</v>
       </c>
@@ -2913,7 +2951,7 @@
       </c>
       <c r="AB14" s="157"/>
     </row>
-    <row r="15" spans="1:29">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>43</v>
       </c>
@@ -3002,7 +3040,7 @@
       </c>
       <c r="AB15" s="157"/>
     </row>
-    <row r="16" spans="1:29" ht="15.75" thickBot="1">
+    <row r="16" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>54</v>
       </c>
@@ -3091,7 +3129,7 @@
       </c>
       <c r="AB16" s="157"/>
     </row>
-    <row r="17" spans="1:28" ht="15.75" thickBot="1">
+    <row r="17" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D17" s="26"/>
       <c r="G17" s="18">
         <f t="shared" si="0"/>
@@ -3174,7 +3212,7 @@
       </c>
       <c r="AB17" s="157"/>
     </row>
-    <row r="18" spans="1:28" ht="15.75" thickBot="1">
+    <row r="18" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="165" t="s">
         <v>73</v>
       </c>
@@ -3261,7 +3299,7 @@
       </c>
       <c r="AB18" s="157"/>
     </row>
-    <row r="19" spans="1:28" ht="15.75" thickBot="1">
+    <row r="19" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="167" t="s">
         <v>58</v>
       </c>
@@ -3348,7 +3386,7 @@
       </c>
       <c r="AB19" s="157"/>
     </row>
-    <row r="20" spans="1:28">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
         <v>60</v>
       </c>
@@ -3441,7 +3479,7 @@
       </c>
       <c r="AB20" s="157"/>
     </row>
-    <row r="21" spans="1:28">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>61</v>
       </c>
@@ -3534,7 +3572,7 @@
       </c>
       <c r="AB21" s="157"/>
     </row>
-    <row r="22" spans="1:28">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>62</v>
       </c>
@@ -3627,7 +3665,7 @@
       </c>
       <c r="AB22" s="157"/>
     </row>
-    <row r="23" spans="1:28">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>63</v>
       </c>
@@ -3720,7 +3758,7 @@
       </c>
       <c r="AB23" s="157"/>
     </row>
-    <row r="24" spans="1:28">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>64</v>
       </c>
@@ -3813,7 +3851,7 @@
       </c>
       <c r="AB24" s="157"/>
     </row>
-    <row r="25" spans="1:28">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>65</v>
       </c>
@@ -3906,7 +3944,7 @@
       </c>
       <c r="AB25" s="157"/>
     </row>
-    <row r="26" spans="1:28">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>66</v>
       </c>
@@ -3999,7 +4037,7 @@
       </c>
       <c r="AB26" s="157"/>
     </row>
-    <row r="27" spans="1:28">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>67</v>
       </c>
@@ -4092,7 +4130,7 @@
       </c>
       <c r="AB27" s="157"/>
     </row>
-    <row r="28" spans="1:28" ht="15.75" thickBot="1">
+    <row r="28" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="27" t="s">
         <v>68</v>
       </c>
@@ -4185,7 +4223,7 @@
       </c>
       <c r="AB28" s="157"/>
     </row>
-    <row r="29" spans="1:28" ht="15.75" thickBot="1">
+    <row r="29" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D29" s="26"/>
       <c r="G29" s="18">
         <f t="shared" si="0"/>
@@ -4268,7 +4306,7 @@
       </c>
       <c r="AB29" s="157"/>
     </row>
-    <row r="30" spans="1:28" ht="15.75" thickBot="1">
+    <row r="30" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="165" t="s">
         <v>69</v>
       </c>
@@ -4355,7 +4393,7 @@
       </c>
       <c r="AB30" s="157"/>
     </row>
-    <row r="31" spans="1:28" ht="15.75" thickBot="1">
+    <row r="31" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="28" t="s">
         <v>70</v>
       </c>
@@ -4448,7 +4486,7 @@
       </c>
       <c r="AB31" s="157"/>
     </row>
-    <row r="32" spans="1:28" ht="15.75" thickBot="1">
+    <row r="32" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D32" s="30"/>
       <c r="G32" s="18">
         <f t="shared" si="0"/>
@@ -4531,7 +4569,7 @@
       </c>
       <c r="AB32" s="157"/>
     </row>
-    <row r="33" spans="1:28" ht="15.75" thickBot="1">
+    <row r="33" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="28" t="s">
         <v>71</v>
       </c>
@@ -4620,7 +4658,7 @@
       </c>
       <c r="AB33" s="157"/>
     </row>
-    <row r="34" spans="1:28" ht="15.75" thickBot="1">
+    <row r="34" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D34" s="30"/>
       <c r="G34" s="18">
         <f t="shared" si="0"/>
@@ -4703,7 +4741,7 @@
       </c>
       <c r="AB34" s="157"/>
     </row>
-    <row r="35" spans="1:28" ht="15.75" thickBot="1">
+    <row r="35" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="28" t="s">
         <v>128</v>
       </c>
@@ -4792,7 +4830,7 @@
       </c>
       <c r="AB35" s="157"/>
     </row>
-    <row r="36" spans="1:28" ht="15.75" thickBot="1">
+    <row r="36" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="28" t="s">
         <v>129</v>
       </c>
@@ -4881,7 +4919,7 @@
       </c>
       <c r="AB36" s="157"/>
     </row>
-    <row r="37" spans="1:28">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D37" s="30"/>
       <c r="G37" s="18">
         <f t="shared" si="0"/>
@@ -4964,7 +5002,7 @@
       </c>
       <c r="AB37" s="157"/>
     </row>
-    <row r="38" spans="1:28">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D38" s="30"/>
       <c r="G38" s="18">
         <f t="shared" si="0"/>
@@ -5047,7 +5085,7 @@
       </c>
       <c r="AB38" s="157"/>
     </row>
-    <row r="39" spans="1:28">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D39" s="30"/>
       <c r="G39" s="18">
         <f t="shared" si="0"/>
@@ -5130,7 +5168,7 @@
       </c>
       <c r="AB39" s="157"/>
     </row>
-    <row r="40" spans="1:28">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D40" s="30"/>
       <c r="G40" s="18">
         <f t="shared" ref="G40:O67" si="6">IF(G$5=0,"",($P40*60*$E$9)/(G$5*63360))</f>
@@ -5213,7 +5251,7 @@
       </c>
       <c r="AB40" s="157"/>
     </row>
-    <row r="41" spans="1:28">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
       <c r="G41" s="18">
         <f t="shared" si="6"/>
         <v>14.931993579922306</v>
@@ -5295,7 +5333,7 @@
       </c>
       <c r="AB41" s="157"/>
     </row>
-    <row r="42" spans="1:28">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
       <c r="G42" s="18">
         <f t="shared" si="6"/>
         <v>15.371169861684725</v>
@@ -5377,7 +5415,7 @@
       </c>
       <c r="AB42" s="157"/>
     </row>
-    <row r="43" spans="1:28">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
       <c r="G43" s="18">
         <f t="shared" si="6"/>
         <v>15.810346143447147</v>
@@ -5459,7 +5497,7 @@
       </c>
       <c r="AB43" s="157"/>
     </row>
-    <row r="44" spans="1:28">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
       <c r="G44" s="18">
         <f t="shared" si="6"/>
         <v>16.249522425209566</v>
@@ -5541,7 +5579,7 @@
       </c>
       <c r="AB44" s="157"/>
     </row>
-    <row r="45" spans="1:28">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
       <c r="G45" s="18">
         <f t="shared" si="6"/>
         <v>16.688698706971987</v>
@@ -5623,7 +5661,7 @@
       </c>
       <c r="AB45" s="157"/>
     </row>
-    <row r="46" spans="1:28">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
       <c r="G46" s="18">
         <f t="shared" si="6"/>
         <v>17.127874988734408</v>
@@ -5705,7 +5743,7 @@
       </c>
       <c r="AB46" s="157"/>
     </row>
-    <row r="47" spans="1:28">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
       <c r="G47" s="18">
         <f t="shared" si="6"/>
         <v>17.56705127049683</v>
@@ -5787,7 +5825,7 @@
       </c>
       <c r="AB47" s="157"/>
     </row>
-    <row r="48" spans="1:28">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
       <c r="G48" s="18">
         <f t="shared" si="6"/>
         <v>18.006227552259251</v>
@@ -5869,7 +5907,7 @@
       </c>
       <c r="AB48" s="157"/>
     </row>
-    <row r="49" spans="7:28">
+    <row r="49" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G49" s="18">
         <f t="shared" si="6"/>
         <v>18.445403834021672</v>
@@ -5951,7 +5989,7 @@
       </c>
       <c r="AB49" s="157"/>
     </row>
-    <row r="50" spans="7:28">
+    <row r="50" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G50" s="18">
         <f t="shared" si="6"/>
         <v>18.88458011578409</v>
@@ -6033,7 +6071,7 @@
       </c>
       <c r="AB50" s="157"/>
     </row>
-    <row r="51" spans="7:28">
+    <row r="51" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G51" s="18">
         <f t="shared" si="6"/>
         <v>19.323756397546511</v>
@@ -6115,7 +6153,7 @@
       </c>
       <c r="AB51" s="157"/>
     </row>
-    <row r="52" spans="7:28">
+    <row r="52" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G52" s="18">
         <f t="shared" si="6"/>
         <v>19.762932679308935</v>
@@ -6197,7 +6235,7 @@
       </c>
       <c r="AB52" s="157"/>
     </row>
-    <row r="53" spans="7:28">
+    <row r="53" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G53" s="18">
         <f t="shared" si="6"/>
         <v>20.202108961071353</v>
@@ -6279,7 +6317,7 @@
       </c>
       <c r="AB53" s="157"/>
     </row>
-    <row r="54" spans="7:28">
+    <row r="54" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G54" s="18">
         <f t="shared" si="6"/>
         <v>20.641285242833774</v>
@@ -6361,7 +6399,7 @@
       </c>
       <c r="AB54" s="157"/>
     </row>
-    <row r="55" spans="7:28">
+    <row r="55" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G55" s="18">
         <f t="shared" si="6"/>
         <v>21.080461524596195</v>
@@ -6443,7 +6481,7 @@
       </c>
       <c r="AB55" s="157"/>
     </row>
-    <row r="56" spans="7:28">
+    <row r="56" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G56" s="18">
         <f t="shared" si="6"/>
         <v>21.519637806358617</v>
@@ -6525,7 +6563,7 @@
       </c>
       <c r="AB56" s="157"/>
     </row>
-    <row r="57" spans="7:28">
+    <row r="57" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G57" s="18">
         <f t="shared" si="6"/>
         <v>21.958814088121034</v>
@@ -6607,7 +6645,7 @@
       </c>
       <c r="AB57" s="157"/>
     </row>
-    <row r="58" spans="7:28">
+    <row r="58" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G58" s="18">
         <f t="shared" si="6"/>
         <v>22.397990369883459</v>
@@ -6689,7 +6727,7 @@
       </c>
       <c r="AB58" s="157"/>
     </row>
-    <row r="59" spans="7:28">
+    <row r="59" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G59" s="18">
         <f t="shared" si="6"/>
         <v>22.83716665164588</v>
@@ -6771,7 +6809,7 @@
       </c>
       <c r="AB59" s="157"/>
     </row>
-    <row r="60" spans="7:28">
+    <row r="60" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G60" s="18">
         <f t="shared" si="6"/>
         <v>23.276342933408298</v>
@@ -6853,7 +6891,7 @@
       </c>
       <c r="AB60" s="157"/>
     </row>
-    <row r="61" spans="7:28">
+    <row r="61" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G61" s="18">
         <f t="shared" si="6"/>
         <v>23.715519215170719</v>
@@ -6935,7 +6973,7 @@
       </c>
       <c r="AB61" s="157"/>
     </row>
-    <row r="62" spans="7:28">
+    <row r="62" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G62" s="18">
         <f t="shared" si="6"/>
         <v>24.15469549693314</v>
@@ -7017,7 +7055,7 @@
       </c>
       <c r="AB62" s="157"/>
     </row>
-    <row r="63" spans="7:28">
+    <row r="63" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G63" s="18">
         <f t="shared" si="6"/>
         <v>24.593871778695561</v>
@@ -7099,7 +7137,7 @@
       </c>
       <c r="AB63" s="157"/>
     </row>
-    <row r="64" spans="7:28">
+    <row r="64" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G64" s="18">
         <f t="shared" si="6"/>
         <v>25.033048060457983</v>
@@ -7181,7 +7219,7 @@
       </c>
       <c r="AB64" s="157"/>
     </row>
-    <row r="65" spans="1:28">
+    <row r="65" spans="1:28" x14ac:dyDescent="0.25">
       <c r="G65" s="18">
         <f t="shared" si="6"/>
         <v>25.472224342220404</v>
@@ -7263,7 +7301,7 @@
       </c>
       <c r="AB65" s="157"/>
     </row>
-    <row r="66" spans="1:28">
+    <row r="66" spans="1:28" x14ac:dyDescent="0.25">
       <c r="G66" s="18">
         <f t="shared" si="6"/>
         <v>25.911400623982825</v>
@@ -7345,7 +7383,7 @@
       </c>
       <c r="AB66" s="157"/>
     </row>
-    <row r="67" spans="1:28" ht="15.75" thickBot="1">
+    <row r="67" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G67" s="18">
         <f t="shared" si="6"/>
         <v>26.350576905745243</v>
@@ -7427,7 +7465,7 @@
       </c>
       <c r="AB67" s="158"/>
     </row>
-    <row r="78" spans="1:28">
+    <row r="78" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>72</v>
       </c>
@@ -7474,47 +7512,48 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AU67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AW67"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S42" activeCellId="1" sqref="S14:S36 S42:S64"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="6.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="3" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="18" width="4" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.7109375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5" style="1" customWidth="1"/>
-    <col min="24" max="29" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="37" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="48" max="16384" width="6.140625" style="1"/>
+    <col min="20" max="21" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="2" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="3" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="33" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="37" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="5.5703125" style="1" customWidth="1"/>
+    <col min="39" max="39" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="5.5703125" style="1" customWidth="1"/>
+    <col min="41" max="41" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="16384" width="6.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A1" s="178" t="s">
+    <row r="1" spans="1:49" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="169" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="179"/>
+      <c r="B1" s="170"/>
     </row>
-    <row r="2" spans="1:47" ht="15.75" thickBot="1">
+    <row r="2" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="81" t="s">
         <v>132</v>
       </c>
@@ -7522,14 +7561,14 @@
         <v>35.86</v>
       </c>
     </row>
-    <row r="3" spans="1:47" ht="15.75" thickBot="1"/>
-    <row r="4" spans="1:47" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A4" s="178" t="s">
+    <row r="3" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:49" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="169" t="s">
         <v>134</v>
       </c>
-      <c r="B4" s="179"/>
+      <c r="B4" s="170"/>
     </row>
-    <row r="5" spans="1:47" ht="15.75" thickBot="1">
+    <row r="5" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="81" t="s">
         <v>21</v>
       </c>
@@ -7537,14 +7576,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:47" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:47" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A7" s="178" t="s">
+    <row r="6" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:49" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="169" t="s">
         <v>135</v>
       </c>
-      <c r="B7" s="179"/>
+      <c r="B7" s="170"/>
     </row>
-    <row r="8" spans="1:47" ht="15.75" thickBot="1">
+    <row r="8" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="81" t="s">
         <v>33</v>
       </c>
@@ -7552,14 +7591,14 @@
         <v>33.299999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:47" ht="15.75" thickBot="1"/>
-    <row r="10" spans="1:47" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A10" s="178" t="s">
+    <row r="9" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:49" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="169" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="179"/>
+      <c r="B10" s="170"/>
     </row>
-    <row r="11" spans="1:47" ht="15.75" thickBot="1">
+    <row r="11" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="81" t="s">
         <v>136</v>
       </c>
@@ -7567,122 +7606,130 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:47" ht="15.75" thickBot="1"/>
-    <row r="13" spans="1:47" ht="15.75" thickBot="1">
-      <c r="A13" s="172" t="s">
+    <row r="12" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="180" t="s">
         <v>137</v>
       </c>
-      <c r="B13" s="170"/>
-      <c r="C13" s="170"/>
-      <c r="D13" s="170"/>
-      <c r="E13" s="170"/>
-      <c r="F13" s="170"/>
-      <c r="G13" s="170"/>
-      <c r="H13" s="170"/>
-      <c r="I13" s="170"/>
-      <c r="J13" s="170"/>
-      <c r="K13" s="170"/>
-      <c r="L13" s="170"/>
-      <c r="M13" s="170"/>
-      <c r="N13" s="170"/>
-      <c r="O13" s="170"/>
-      <c r="P13" s="170"/>
-      <c r="Q13" s="170"/>
-      <c r="R13" s="170"/>
-      <c r="S13" s="170"/>
-      <c r="T13" s="170"/>
-      <c r="U13" s="170"/>
-      <c r="V13" s="170"/>
-      <c r="W13" s="170"/>
-      <c r="X13" s="170"/>
-      <c r="Y13" s="170"/>
-      <c r="Z13" s="170"/>
-      <c r="AA13" s="170"/>
-      <c r="AB13" s="170"/>
-      <c r="AC13" s="170"/>
-      <c r="AD13" s="170"/>
-      <c r="AE13" s="170"/>
-      <c r="AF13" s="170"/>
-      <c r="AG13" s="170"/>
-      <c r="AH13" s="170"/>
-      <c r="AI13" s="170"/>
-      <c r="AJ13" s="170"/>
-      <c r="AK13" s="171"/>
-      <c r="AM13" s="85" t="s">
+      <c r="B13" s="181"/>
+      <c r="C13" s="181"/>
+      <c r="D13" s="181"/>
+      <c r="E13" s="181"/>
+      <c r="F13" s="181"/>
+      <c r="G13" s="181"/>
+      <c r="H13" s="181"/>
+      <c r="I13" s="181"/>
+      <c r="J13" s="181"/>
+      <c r="K13" s="181"/>
+      <c r="L13" s="181"/>
+      <c r="M13" s="181"/>
+      <c r="N13" s="181"/>
+      <c r="O13" s="181"/>
+      <c r="P13" s="181"/>
+      <c r="Q13" s="181"/>
+      <c r="R13" s="181"/>
+      <c r="S13" s="181"/>
+      <c r="T13" s="181"/>
+      <c r="U13" s="181"/>
+      <c r="V13" s="181"/>
+      <c r="W13" s="181"/>
+      <c r="X13" s="181"/>
+      <c r="Y13" s="181"/>
+      <c r="Z13" s="181"/>
+      <c r="AA13" s="181"/>
+      <c r="AB13" s="181"/>
+      <c r="AC13" s="181"/>
+      <c r="AD13" s="181"/>
+      <c r="AE13" s="181"/>
+      <c r="AF13" s="181"/>
+      <c r="AG13" s="181"/>
+      <c r="AH13" s="181"/>
+      <c r="AI13" s="181"/>
+      <c r="AJ13" s="181"/>
+      <c r="AK13" s="181"/>
+      <c r="AL13" s="181"/>
+      <c r="AM13" s="182"/>
+      <c r="AO13" s="85" t="s">
         <v>131</v>
       </c>
-      <c r="AN13" s="85"/>
-      <c r="AO13" s="85"/>
       <c r="AP13" s="85"/>
       <c r="AQ13" s="85"/>
       <c r="AR13" s="85"/>
       <c r="AS13" s="85"/>
       <c r="AT13" s="85"/>
       <c r="AU13" s="85"/>
+      <c r="AV13" s="85"/>
+      <c r="AW13" s="85"/>
     </row>
-    <row r="14" spans="1:47">
-      <c r="A14" s="172" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="170"/>
-      <c r="C14" s="170" t="s">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A14" s="174" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="176"/>
+      <c r="C14" s="176" t="s">
         <v>138</v>
       </c>
-      <c r="D14" s="170"/>
-      <c r="E14" s="170"/>
-      <c r="F14" s="170"/>
-      <c r="G14" s="170"/>
-      <c r="H14" s="170"/>
-      <c r="I14" s="170"/>
-      <c r="J14" s="170"/>
-      <c r="K14" s="170"/>
-      <c r="L14" s="170"/>
-      <c r="M14" s="170"/>
-      <c r="N14" s="170"/>
-      <c r="O14" s="170"/>
-      <c r="P14" s="170"/>
-      <c r="Q14" s="170"/>
-      <c r="R14" s="171"/>
-      <c r="S14" s="121" t="s">
+      <c r="D14" s="176"/>
+      <c r="E14" s="176"/>
+      <c r="F14" s="176"/>
+      <c r="G14" s="176"/>
+      <c r="H14" s="176"/>
+      <c r="I14" s="176"/>
+      <c r="J14" s="176"/>
+      <c r="K14" s="176"/>
+      <c r="L14" s="176"/>
+      <c r="M14" s="176"/>
+      <c r="N14" s="176"/>
+      <c r="O14" s="176"/>
+      <c r="P14" s="176"/>
+      <c r="Q14" s="176"/>
+      <c r="R14" s="184"/>
+      <c r="S14" s="127" t="s">
         <v>141</v>
       </c>
-      <c r="T14" s="172" t="s">
+      <c r="T14" s="174" t="s">
         <v>107</v>
       </c>
-      <c r="U14" s="170"/>
-      <c r="V14" s="170" t="s">
+      <c r="U14" s="176"/>
+      <c r="V14" s="176" t="s">
         <v>12</v>
       </c>
-      <c r="W14" s="170"/>
-      <c r="X14" s="170"/>
-      <c r="Y14" s="170"/>
-      <c r="Z14" s="170"/>
-      <c r="AA14" s="170"/>
-      <c r="AB14" s="170"/>
-      <c r="AC14" s="170"/>
-      <c r="AD14" s="170"/>
-      <c r="AE14" s="170"/>
-      <c r="AF14" s="170"/>
-      <c r="AG14" s="170"/>
-      <c r="AH14" s="170"/>
-      <c r="AI14" s="170"/>
-      <c r="AJ14" s="170"/>
-      <c r="AK14" s="171"/>
-      <c r="AM14" s="85"/>
-      <c r="AN14" s="169" t="s">
+      <c r="W14" s="176"/>
+      <c r="X14" s="176"/>
+      <c r="Y14" s="176"/>
+      <c r="Z14" s="176"/>
+      <c r="AA14" s="176"/>
+      <c r="AB14" s="176"/>
+      <c r="AC14" s="176"/>
+      <c r="AD14" s="176"/>
+      <c r="AE14" s="176"/>
+      <c r="AF14" s="176"/>
+      <c r="AG14" s="176"/>
+      <c r="AH14" s="176"/>
+      <c r="AI14" s="176"/>
+      <c r="AJ14" s="176"/>
+      <c r="AK14" s="184"/>
+      <c r="AL14" s="192" t="s">
+        <v>6</v>
+      </c>
+      <c r="AM14" s="190" t="s">
+        <v>149</v>
+      </c>
+      <c r="AO14" s="85"/>
+      <c r="AP14" s="179" t="s">
         <v>31</v>
       </c>
-      <c r="AO14" s="169"/>
-      <c r="AP14" s="169"/>
-      <c r="AQ14" s="169"/>
-      <c r="AR14" s="169"/>
-      <c r="AS14" s="169"/>
-      <c r="AT14" s="169"/>
-      <c r="AU14" s="169"/>
+      <c r="AQ14" s="179"/>
+      <c r="AR14" s="179"/>
+      <c r="AS14" s="179"/>
+      <c r="AT14" s="179"/>
+      <c r="AU14" s="179"/>
+      <c r="AV14" s="179"/>
+      <c r="AW14" s="179"/>
     </row>
-    <row r="15" spans="1:47" ht="15.75" thickBot="1">
-      <c r="A15" s="173"/>
-      <c r="B15" s="174"/>
+    <row r="15" spans="1:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="174"/>
+      <c r="B15" s="176"/>
       <c r="C15" s="102">
         <v>0</v>
       </c>
@@ -7732,8 +7779,8 @@
         <v>140</v>
       </c>
       <c r="S15" s="122"/>
-      <c r="T15" s="173"/>
-      <c r="U15" s="174"/>
+      <c r="T15" s="174"/>
+      <c r="U15" s="176"/>
       <c r="V15" s="10">
         <f>C15</f>
         <v>0</v>
@@ -7798,36 +7845,40 @@
         <f t="shared" si="0"/>
         <v>140</v>
       </c>
-      <c r="AM15" s="85" t="s">
+      <c r="AL15" s="193"/>
+      <c r="AM15" s="191">
+        <v>650</v>
+      </c>
+      <c r="AO15" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="AN15" s="85" t="s">
+      <c r="AP15" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="AO15" s="85" t="s">
+      <c r="AQ15" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="AP15" s="85" t="s">
+      <c r="AR15" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="AQ15" s="85" t="s">
+      <c r="AS15" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="AR15" s="85" t="s">
+      <c r="AT15" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="AS15" s="85" t="s">
+      <c r="AU15" s="85" t="s">
         <v>23</v>
       </c>
-      <c r="AT15" s="85" t="s">
+      <c r="AV15" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="AU15" s="86" t="s">
+      <c r="AW15" s="86" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:47">
-      <c r="A16" s="173" t="s">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A16" s="174" t="s">
         <v>139</v>
       </c>
       <c r="B16" s="102">
@@ -7898,7 +7949,7 @@
         <v>69.499247954941652</v>
       </c>
       <c r="S16" s="122"/>
-      <c r="T16" s="173" t="s">
+      <c r="T16" s="174" t="s">
         <v>5</v>
       </c>
       <c r="U16" s="10">
@@ -7969,36 +8020,41 @@
         <f t="shared" si="2"/>
         <v>588.73856799280998</v>
       </c>
-      <c r="AM16" s="85" t="s">
+      <c r="AL16" s="193"/>
+      <c r="AM16" s="188">
+        <f>$AM$15/((1/1)*(1/745.7)*($B$2/1)*($B$5/1)*($B16/1)*(1/60)*($B$8/100))</f>
+        <v>1309.3666863704468</v>
+      </c>
+      <c r="AO16" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="AN16" s="85" t="s">
+      <c r="AP16" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="AO16" s="85" t="s">
+      <c r="AQ16" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="AP16" s="85" t="s">
+      <c r="AR16" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="AQ16" s="85" t="s">
+      <c r="AS16" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="AR16" s="85" t="s">
+      <c r="AT16" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="AS16" s="85" t="s">
+      <c r="AU16" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="AT16" s="85" t="s">
+      <c r="AV16" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="AU16" s="86">
+      <c r="AW16" s="86">
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:47">
-      <c r="A17" s="173"/>
+    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A17" s="174"/>
       <c r="B17" s="105">
         <v>650</v>
       </c>
@@ -8067,7 +8123,7 @@
         <v>72.862114791471072</v>
       </c>
       <c r="S17" s="122"/>
-      <c r="T17" s="173"/>
+      <c r="T17" s="174"/>
       <c r="U17" s="10">
         <f t="shared" ref="U17:U36" si="3">B17</f>
         <v>650</v>
@@ -8136,8 +8192,11 @@
         <f t="shared" si="2"/>
         <v>588.73856799280986</v>
       </c>
-      <c r="AM17" s="85"/>
-      <c r="AN17" s="85"/>
+      <c r="AL17" s="193"/>
+      <c r="AM17" s="188">
+        <f>$AM$15/((1/1)*(1/745.7)*($B$2/1)*($B$5/1)*($B17/1)*(1/60)*($B$8/100))</f>
+        <v>1248.9343777687341</v>
+      </c>
       <c r="AO17" s="85"/>
       <c r="AP17" s="85"/>
       <c r="AQ17" s="85"/>
@@ -8145,9 +8204,11 @@
       <c r="AS17" s="85"/>
       <c r="AT17" s="85"/>
       <c r="AU17" s="85"/>
+      <c r="AV17" s="85"/>
+      <c r="AW17" s="85"/>
     </row>
-    <row r="18" spans="1:47">
-      <c r="A18" s="173"/>
+    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A18" s="174"/>
       <c r="B18" s="105">
         <v>800</v>
       </c>
@@ -8216,7 +8277,7 @@
         <v>89.676448974118259</v>
       </c>
       <c r="S18" s="122"/>
-      <c r="T18" s="173"/>
+      <c r="T18" s="174"/>
       <c r="U18" s="10">
         <f t="shared" si="3"/>
         <v>800</v>
@@ -8285,20 +8346,25 @@
         <f t="shared" si="2"/>
         <v>588.73856799280998</v>
       </c>
-      <c r="AM18" s="85"/>
-      <c r="AN18" s="169" t="s">
+      <c r="AL18" s="193"/>
+      <c r="AM18" s="188">
+        <f>$AM$15/((1/1)*(1/745.7)*($B$2/1)*($B$5/1)*($B18/1)*(1/60)*($B$8/100))</f>
+        <v>1014.7591819370965</v>
+      </c>
+      <c r="AO18" s="85"/>
+      <c r="AP18" s="179" t="s">
         <v>32</v>
       </c>
-      <c r="AO18" s="169"/>
-      <c r="AP18" s="169"/>
-      <c r="AQ18" s="85"/>
-      <c r="AR18" s="85"/>
+      <c r="AQ18" s="179"/>
+      <c r="AR18" s="179"/>
       <c r="AS18" s="85"/>
       <c r="AT18" s="85"/>
-      <c r="AU18" s="86"/>
+      <c r="AU18" s="85"/>
+      <c r="AV18" s="85"/>
+      <c r="AW18" s="86"/>
     </row>
-    <row r="19" spans="1:47">
-      <c r="A19" s="173"/>
+    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A19" s="174"/>
       <c r="B19" s="105">
         <v>1000</v>
       </c>
@@ -8367,7 +8433,7 @@
         <v>112.09556121764783</v>
       </c>
       <c r="S19" s="122"/>
-      <c r="T19" s="173"/>
+      <c r="T19" s="174"/>
       <c r="U19" s="10">
         <f t="shared" si="3"/>
         <v>1000</v>
@@ -8436,24 +8502,29 @@
         <f t="shared" si="2"/>
         <v>588.73856799281009</v>
       </c>
-      <c r="AM19" s="85" t="s">
+      <c r="AL19" s="193"/>
+      <c r="AM19" s="188">
+        <f>$AM$15/((1/1)*(1/745.7)*($B$2/1)*($B$5/1)*($B19/1)*(1/60)*($B$8/100))</f>
+        <v>811.80734554967705</v>
+      </c>
+      <c r="AO19" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="AN19" s="85" t="s">
-        <v>0</v>
-      </c>
-      <c r="AO19" s="85">
+      <c r="AP19" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ19" s="85">
         <v>5252.1131220325396</v>
       </c>
-      <c r="AP19" s="85"/>
-      <c r="AQ19" s="85"/>
       <c r="AR19" s="85"/>
       <c r="AS19" s="85"/>
       <c r="AT19" s="85"/>
-      <c r="AU19" s="86"/>
+      <c r="AU19" s="85"/>
+      <c r="AV19" s="85"/>
+      <c r="AW19" s="86"/>
     </row>
-    <row r="20" spans="1:47">
-      <c r="A20" s="173"/>
+    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A20" s="174"/>
       <c r="B20" s="105">
         <v>1200</v>
       </c>
@@ -8522,7 +8593,7 @@
         <v>134.51467346117738</v>
       </c>
       <c r="S20" s="122"/>
-      <c r="T20" s="173"/>
+      <c r="T20" s="174"/>
       <c r="U20" s="10">
         <f t="shared" si="3"/>
         <v>1200</v>
@@ -8591,22 +8662,27 @@
         <f t="shared" si="2"/>
         <v>588.73856799280998</v>
       </c>
-      <c r="AM20" s="85" t="s">
+      <c r="AL20" s="193"/>
+      <c r="AM20" s="188">
+        <f>$AM$15/((1/1)*(1/745.7)*($B$2/1)*($B$5/1)*($B20/1)*(1/60)*($B$8/100))</f>
+        <v>676.50612129139756</v>
+      </c>
+      <c r="AO20" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="AN20" s="85"/>
-      <c r="AO20" s="85"/>
-      <c r="AP20" s="85" t="s">
+      <c r="AP20" s="85"/>
+      <c r="AQ20" s="85"/>
+      <c r="AR20" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="AQ20" s="85"/>
-      <c r="AR20" s="85"/>
       <c r="AS20" s="85"/>
       <c r="AT20" s="85"/>
       <c r="AU20" s="85"/>
+      <c r="AV20" s="85"/>
+      <c r="AW20" s="85"/>
     </row>
-    <row r="21" spans="1:47">
-      <c r="A21" s="173"/>
+    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A21" s="174"/>
       <c r="B21" s="105">
         <v>1400</v>
       </c>
@@ -8675,7 +8751,7 @@
         <v>156.93378570470696</v>
       </c>
       <c r="S21" s="122"/>
-      <c r="T21" s="173"/>
+      <c r="T21" s="174"/>
       <c r="U21" s="10">
         <f t="shared" si="3"/>
         <v>1400</v>
@@ -8744,9 +8820,14 @@
         <f t="shared" si="2"/>
         <v>588.73856799280998</v>
       </c>
+      <c r="AL21" s="193"/>
+      <c r="AM21" s="188">
+        <f>$AM$15/((1/1)*(1/745.7)*($B$2/1)*($B$5/1)*($B21/1)*(1/60)*($B$8/100))</f>
+        <v>579.86238967834083</v>
+      </c>
     </row>
-    <row r="22" spans="1:47">
-      <c r="A22" s="173"/>
+    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A22" s="174"/>
       <c r="B22" s="105">
         <v>1550</v>
       </c>
@@ -8815,7 +8896,7 @@
         <v>173.74811988735411</v>
       </c>
       <c r="S22" s="122"/>
-      <c r="T22" s="173"/>
+      <c r="T22" s="174"/>
       <c r="U22" s="10">
         <f t="shared" si="3"/>
         <v>1550</v>
@@ -8884,9 +8965,14 @@
         <f t="shared" si="2"/>
         <v>588.73856799280998</v>
       </c>
+      <c r="AL22" s="193"/>
+      <c r="AM22" s="188">
+        <f>$AM$15/((1/1)*(1/745.7)*($B$2/1)*($B$5/1)*($B22/1)*(1/60)*($B$8/100))</f>
+        <v>523.74667454817882</v>
+      </c>
     </row>
-    <row r="23" spans="1:47">
-      <c r="A23" s="173"/>
+    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A23" s="174"/>
       <c r="B23" s="105">
         <v>1700</v>
       </c>
@@ -8955,7 +9041,7 @@
         <v>190.56245407000131</v>
       </c>
       <c r="S23" s="122"/>
-      <c r="T23" s="173"/>
+      <c r="T23" s="174"/>
       <c r="U23" s="10">
         <f t="shared" si="3"/>
         <v>1700</v>
@@ -9024,9 +9110,14 @@
         <f t="shared" si="2"/>
         <v>588.73856799281009</v>
       </c>
+      <c r="AL23" s="193"/>
+      <c r="AM23" s="188">
+        <f>$AM$15/((1/1)*(1/745.7)*($B$2/1)*($B$5/1)*($B23/1)*(1/60)*($B$8/100))</f>
+        <v>477.53373267628064</v>
+      </c>
     </row>
-    <row r="24" spans="1:47">
-      <c r="A24" s="173"/>
+    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A24" s="174"/>
       <c r="B24" s="105">
         <v>1800</v>
       </c>
@@ -9095,7 +9186,7 @@
         <v>201.77201019176607</v>
       </c>
       <c r="S24" s="122"/>
-      <c r="T24" s="173"/>
+      <c r="T24" s="174"/>
       <c r="U24" s="10">
         <f t="shared" si="3"/>
         <v>1800</v>
@@ -9164,9 +9255,14 @@
         <f t="shared" si="2"/>
         <v>588.73856799280998</v>
       </c>
+      <c r="AL24" s="193"/>
+      <c r="AM24" s="188">
+        <f>$AM$15/((1/1)*(1/745.7)*($B$2/1)*($B$5/1)*($B24/1)*(1/60)*($B$8/100))</f>
+        <v>451.00408086093171</v>
+      </c>
     </row>
-    <row r="25" spans="1:47">
-      <c r="A25" s="173"/>
+    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A25" s="174"/>
       <c r="B25" s="105">
         <v>2000</v>
       </c>
@@ -9235,7 +9331,7 @@
         <v>224.19112243529565</v>
       </c>
       <c r="S25" s="122"/>
-      <c r="T25" s="173"/>
+      <c r="T25" s="174"/>
       <c r="U25" s="10">
         <f t="shared" si="3"/>
         <v>2000</v>
@@ -9304,9 +9400,14 @@
         <f t="shared" si="2"/>
         <v>588.73856799281009</v>
       </c>
+      <c r="AL25" s="193"/>
+      <c r="AM25" s="188">
+        <f>$AM$15/((1/1)*(1/745.7)*($B$2/1)*($B$5/1)*($B25/1)*(1/60)*($B$8/100))</f>
+        <v>405.90367277483853</v>
+      </c>
     </row>
-    <row r="26" spans="1:47">
-      <c r="A26" s="173"/>
+    <row r="26" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A26" s="174"/>
       <c r="B26" s="105">
         <v>2200</v>
       </c>
@@ -9375,7 +9476,7 @@
         <v>246.61023467882521</v>
       </c>
       <c r="S26" s="122"/>
-      <c r="T26" s="173"/>
+      <c r="T26" s="174"/>
       <c r="U26" s="10">
         <f t="shared" si="3"/>
         <v>2200</v>
@@ -9444,9 +9545,14 @@
         <f t="shared" si="5"/>
         <v>588.73856799280998</v>
       </c>
+      <c r="AL26" s="193"/>
+      <c r="AM26" s="188">
+        <f>$AM$15/((1/1)*(1/745.7)*($B$2/1)*($B$5/1)*($B26/1)*(1/60)*($B$8/100))</f>
+        <v>369.0033388862168</v>
+      </c>
     </row>
-    <row r="27" spans="1:47">
-      <c r="A27" s="173"/>
+    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A27" s="174"/>
       <c r="B27" s="105">
         <v>2400</v>
       </c>
@@ -9515,7 +9621,7 @@
         <v>269.02934692235476</v>
       </c>
       <c r="S27" s="122"/>
-      <c r="T27" s="173"/>
+      <c r="T27" s="174"/>
       <c r="U27" s="10">
         <f t="shared" si="3"/>
         <v>2400</v>
@@ -9584,9 +9690,14 @@
         <f t="shared" si="5"/>
         <v>588.73856799280998</v>
       </c>
+      <c r="AL27" s="193"/>
+      <c r="AM27" s="188">
+        <f>$AM$15/((1/1)*(1/745.7)*($B$2/1)*($B$5/1)*($B27/1)*(1/60)*($B$8/100))</f>
+        <v>338.25306064569878</v>
+      </c>
     </row>
-    <row r="28" spans="1:47">
-      <c r="A28" s="173"/>
+    <row r="28" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A28" s="174"/>
       <c r="B28" s="105">
         <v>2600</v>
       </c>
@@ -9655,7 +9766,7 @@
         <v>291.44845916588429</v>
       </c>
       <c r="S28" s="122"/>
-      <c r="T28" s="173"/>
+      <c r="T28" s="174"/>
       <c r="U28" s="10">
         <f t="shared" si="3"/>
         <v>2600</v>
@@ -9724,9 +9835,14 @@
         <f t="shared" si="5"/>
         <v>588.73856799280986</v>
       </c>
+      <c r="AL28" s="193"/>
+      <c r="AM28" s="188">
+        <f>$AM$15/((1/1)*(1/745.7)*($B$2/1)*($B$5/1)*($B28/1)*(1/60)*($B$8/100))</f>
+        <v>312.23359444218352</v>
+      </c>
     </row>
-    <row r="29" spans="1:47">
-      <c r="A29" s="173"/>
+    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A29" s="174"/>
       <c r="B29" s="105">
         <v>2800</v>
       </c>
@@ -9795,7 +9911,7 @@
         <v>313.86757140941393</v>
       </c>
       <c r="S29" s="122"/>
-      <c r="T29" s="173"/>
+      <c r="T29" s="174"/>
       <c r="U29" s="10">
         <f t="shared" si="3"/>
         <v>2800</v>
@@ -9864,9 +9980,14 @@
         <f t="shared" si="5"/>
         <v>588.73856799280998</v>
       </c>
+      <c r="AL29" s="193"/>
+      <c r="AM29" s="188">
+        <f>$AM$15/((1/1)*(1/745.7)*($B$2/1)*($B$5/1)*($B29/1)*(1/60)*($B$8/100))</f>
+        <v>289.93119483917042</v>
+      </c>
     </row>
-    <row r="30" spans="1:47">
-      <c r="A30" s="173"/>
+    <row r="30" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A30" s="174"/>
       <c r="B30" s="105">
         <v>2900</v>
       </c>
@@ -9937,7 +10058,7 @@
       <c r="S30" s="122" t="s">
         <v>140</v>
       </c>
-      <c r="T30" s="173"/>
+      <c r="T30" s="174"/>
       <c r="U30" s="10">
         <f t="shared" si="3"/>
         <v>2900</v>
@@ -10006,9 +10127,14 @@
         <f t="shared" si="5"/>
         <v>588.73856799280998</v>
       </c>
+      <c r="AL30" s="193"/>
+      <c r="AM30" s="188">
+        <f>$AM$15/((1/1)*(1/745.7)*($B$2/1)*($B$5/1)*($B30/1)*(1/60)*($B$8/100))</f>
+        <v>279.93356743092318</v>
+      </c>
     </row>
-    <row r="31" spans="1:47">
-      <c r="A31" s="173"/>
+    <row r="31" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A31" s="174"/>
       <c r="B31" s="105">
         <v>3000</v>
       </c>
@@ -10077,7 +10203,7 @@
         <v>336.28668365294345</v>
       </c>
       <c r="S31" s="122"/>
-      <c r="T31" s="173"/>
+      <c r="T31" s="174"/>
       <c r="U31" s="10">
         <f t="shared" si="3"/>
         <v>3000</v>
@@ -10146,9 +10272,14 @@
         <f t="shared" si="5"/>
         <v>588.73856799280998</v>
       </c>
+      <c r="AL31" s="193"/>
+      <c r="AM31" s="188">
+        <f>$AM$15/((1/1)*(1/745.7)*($B$2/1)*($B$5/1)*($B31/1)*(1/60)*($B$8/100))</f>
+        <v>270.60244851655898</v>
+      </c>
     </row>
-    <row r="32" spans="1:47">
-      <c r="A32" s="173"/>
+    <row r="32" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A32" s="174"/>
       <c r="B32" s="105">
         <v>3200</v>
       </c>
@@ -10217,7 +10348,7 @@
         <v>358.70579589647303</v>
       </c>
       <c r="S32" s="122"/>
-      <c r="T32" s="173"/>
+      <c r="T32" s="174"/>
       <c r="U32" s="10">
         <f t="shared" si="3"/>
         <v>3200</v>
@@ -10286,9 +10417,14 @@
         <f t="shared" si="5"/>
         <v>588.73856799280998</v>
       </c>
+      <c r="AL32" s="193"/>
+      <c r="AM32" s="188">
+        <f>$AM$15/((1/1)*(1/745.7)*($B$2/1)*($B$5/1)*($B32/1)*(1/60)*($B$8/100))</f>
+        <v>253.68979548427413</v>
+      </c>
     </row>
-    <row r="33" spans="1:41">
-      <c r="A33" s="173"/>
+    <row r="33" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A33" s="174"/>
       <c r="B33" s="105">
         <v>3300</v>
       </c>
@@ -10357,7 +10493,7 @@
         <v>369.9153520182378</v>
       </c>
       <c r="S33" s="122"/>
-      <c r="T33" s="173"/>
+      <c r="T33" s="174"/>
       <c r="U33" s="10">
         <f t="shared" si="3"/>
         <v>3300</v>
@@ -10426,9 +10562,14 @@
         <f t="shared" si="5"/>
         <v>588.73856799280998</v>
       </c>
+      <c r="AL33" s="193"/>
+      <c r="AM33" s="188">
+        <f>$AM$15/((1/1)*(1/745.7)*($B$2/1)*($B$5/1)*($B33/1)*(1/60)*($B$8/100))</f>
+        <v>246.00222592414454</v>
+      </c>
     </row>
-    <row r="34" spans="1:41">
-      <c r="A34" s="173"/>
+    <row r="34" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A34" s="174"/>
       <c r="B34" s="105">
         <v>3500</v>
       </c>
@@ -10499,7 +10640,7 @@
       <c r="S34" s="122" t="s">
         <v>4</v>
       </c>
-      <c r="T34" s="173"/>
+      <c r="T34" s="174"/>
       <c r="U34" s="10">
         <f t="shared" si="3"/>
         <v>3500</v>
@@ -10568,11 +10709,16 @@
         <f t="shared" si="5"/>
         <v>588.73856799280986</v>
       </c>
+      <c r="AL34" s="193"/>
+      <c r="AM34" s="188">
+        <f>$AM$15/((1/1)*(1/745.7)*($B$2/1)*($B$5/1)*($B34/1)*(1/60)*($B$8/100))</f>
+        <v>231.94495587133628</v>
+      </c>
     </row>
-    <row r="35" spans="1:41">
-      <c r="A35" s="173"/>
+    <row r="35" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A35" s="174"/>
       <c r="B35" s="105">
-        <v>4000</v>
+        <v>3800</v>
       </c>
       <c r="C35" s="71">
         <f t="shared" si="4"/>
@@ -10580,69 +10726,69 @@
       </c>
       <c r="D35" s="64">
         <f t="shared" si="4"/>
-        <v>32.027303205042237</v>
+        <v>30.425938044790122</v>
       </c>
       <c r="E35" s="64">
         <f t="shared" si="4"/>
-        <v>64.054606410084475</v>
+        <v>60.851876089580244</v>
       </c>
       <c r="F35" s="64">
         <f t="shared" si="4"/>
-        <v>96.081909615126705</v>
+        <v>91.277814134370374</v>
       </c>
       <c r="G35" s="64">
         <f t="shared" si="4"/>
-        <v>144.12286442269004</v>
+        <v>136.91672120155556</v>
       </c>
       <c r="H35" s="64">
         <f t="shared" si="4"/>
-        <v>176.15016762773226</v>
+        <v>167.34265924634565</v>
       </c>
       <c r="I35" s="64">
         <f t="shared" si="4"/>
-        <v>208.17747083277447</v>
+        <v>197.76859729113582</v>
       </c>
       <c r="J35" s="64">
         <f t="shared" si="4"/>
-        <v>240.20477403781675</v>
+        <v>228.19453533592588</v>
       </c>
       <c r="K35" s="64">
         <f t="shared" si="4"/>
-        <v>272.23207724285902</v>
+        <v>258.62047338071602</v>
       </c>
       <c r="L35" s="64">
         <f t="shared" si="4"/>
-        <v>304.25938044790121</v>
+        <v>289.04641142550616</v>
       </c>
       <c r="M35" s="64">
         <f t="shared" si="4"/>
-        <v>352.30033525546452</v>
+        <v>334.68531849269129</v>
       </c>
       <c r="N35" s="64">
         <f t="shared" si="4"/>
-        <v>384.32763846050682</v>
+        <v>365.11125653748149</v>
       </c>
       <c r="O35" s="64">
         <f t="shared" si="4"/>
-        <v>400.34129006302794</v>
+        <v>380.32422555987648</v>
       </c>
       <c r="P35" s="64">
         <f t="shared" si="4"/>
-        <v>416.35494166554895</v>
+        <v>395.53719458227164</v>
       </c>
       <c r="Q35" s="64">
         <f t="shared" si="4"/>
-        <v>432.36859326807007</v>
+        <v>410.75016360466662</v>
       </c>
       <c r="R35" s="65">
         <f t="shared" si="4"/>
-        <v>448.38224487059131</v>
+        <v>425.96313262706173</v>
       </c>
       <c r="S35" s="122"/>
-      <c r="T35" s="173"/>
+      <c r="T35" s="174"/>
       <c r="U35" s="10">
         <f t="shared" si="3"/>
-        <v>4000</v>
+        <v>3800</v>
       </c>
       <c r="V35" s="71">
         <f t="shared" si="5"/>
@@ -10650,19 +10796,19 @@
       </c>
       <c r="W35" s="64">
         <f t="shared" si="5"/>
-        <v>42.052754856629292</v>
+        <v>42.052754856629278</v>
       </c>
       <c r="X35" s="64">
         <f t="shared" si="5"/>
-        <v>84.105509713258584</v>
+        <v>84.105509713258556</v>
       </c>
       <c r="Y35" s="64">
         <f t="shared" si="5"/>
-        <v>126.15826456988785</v>
+        <v>126.15826456988786</v>
       </c>
       <c r="Z35" s="64">
         <f t="shared" si="5"/>
-        <v>189.23739685483176</v>
+        <v>189.23739685483179</v>
       </c>
       <c r="AA35" s="64">
         <f t="shared" si="5"/>
@@ -10670,19 +10816,19 @@
       </c>
       <c r="AB35" s="64">
         <f t="shared" si="5"/>
-        <v>273.34290656809026</v>
+        <v>273.34290656809037</v>
       </c>
       <c r="AC35" s="64">
         <f t="shared" si="5"/>
-        <v>315.39566142471961</v>
+        <v>315.39566142471955</v>
       </c>
       <c r="AD35" s="64">
         <f t="shared" si="5"/>
-        <v>357.44841628134895</v>
+        <v>357.4484162813489</v>
       </c>
       <c r="AE35" s="64">
         <f t="shared" si="5"/>
-        <v>399.50117113797813</v>
+        <v>399.50117113797819</v>
       </c>
       <c r="AF35" s="64">
         <f t="shared" si="5"/>
@@ -10690,26 +10836,31 @@
       </c>
       <c r="AG35" s="64">
         <f t="shared" si="5"/>
-        <v>504.63305827955139</v>
+        <v>504.63305827955145</v>
       </c>
       <c r="AH35" s="64">
         <f t="shared" si="5"/>
-        <v>525.65943570786612</v>
+        <v>525.65943570786601</v>
       </c>
       <c r="AI35" s="64">
         <f t="shared" si="5"/>
-        <v>546.68581313618051</v>
+        <v>546.68581313618074</v>
       </c>
       <c r="AJ35" s="64">
         <f t="shared" si="5"/>
-        <v>567.71219056449513</v>
+        <v>567.71219056449524</v>
       </c>
       <c r="AK35" s="65">
         <f t="shared" si="5"/>
-        <v>588.73856799281009</v>
+        <v>588.73856799280998</v>
+      </c>
+      <c r="AL35" s="193"/>
+      <c r="AM35" s="188">
+        <f>$AM$15/((1/1)*(1/745.7)*($B$2/1)*($B$5/1)*($B35/1)*(1/60)*($B$8/100))</f>
+        <v>213.63351198675713</v>
       </c>
     </row>
-    <row r="36" spans="1:41" ht="15.75" thickBot="1">
+    <row r="36" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="175"/>
       <c r="B36" s="106">
         <v>4500</v>
@@ -10848,15 +10999,20 @@
         <f t="shared" si="5"/>
         <v>588.73856799280998</v>
       </c>
+      <c r="AL36" s="194"/>
+      <c r="AM36" s="189">
+        <f>$AM$15/((1/1)*(1/745.7)*($B$2/1)*($B$5/1)*($B36/1)*(1/60)*($B$8/100))</f>
+        <v>180.40163234437264</v>
+      </c>
     </row>
-    <row r="37" spans="1:41" ht="15.75" thickBot="1"/>
-    <row r="38" spans="1:41" ht="15.75" thickBot="1">
-      <c r="A38" s="176" t="s">
+    <row r="37" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="177" t="s">
         <v>116</v>
       </c>
-      <c r="B38" s="177"/>
+      <c r="B38" s="178"/>
     </row>
-    <row r="39" spans="1:41" ht="15.75" thickBot="1">
+    <row r="39" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="28" t="s">
         <v>40</v>
       </c>
@@ -10865,100 +11021,100 @@
         <v>2.9467000000000003</v>
       </c>
     </row>
-    <row r="40" spans="1:41" ht="15.75" thickBot="1"/>
-    <row r="41" spans="1:41" ht="15.75" thickBot="1">
-      <c r="A41" s="172" t="s">
+    <row r="40" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="171" t="s">
         <v>130</v>
       </c>
-      <c r="B41" s="170"/>
-      <c r="C41" s="170"/>
-      <c r="D41" s="170"/>
-      <c r="E41" s="170"/>
-      <c r="F41" s="170"/>
-      <c r="G41" s="170"/>
-      <c r="H41" s="170"/>
-      <c r="I41" s="170"/>
-      <c r="J41" s="170"/>
-      <c r="K41" s="170"/>
-      <c r="L41" s="170"/>
-      <c r="M41" s="170"/>
-      <c r="N41" s="170"/>
-      <c r="O41" s="170"/>
-      <c r="P41" s="170"/>
-      <c r="Q41" s="170"/>
-      <c r="R41" s="170"/>
-      <c r="S41" s="170"/>
-      <c r="T41" s="170"/>
-      <c r="U41" s="170"/>
-      <c r="V41" s="170"/>
-      <c r="W41" s="170"/>
-      <c r="X41" s="170"/>
-      <c r="Y41" s="170"/>
-      <c r="Z41" s="170"/>
-      <c r="AA41" s="170"/>
-      <c r="AB41" s="170"/>
-      <c r="AC41" s="170"/>
-      <c r="AD41" s="170"/>
-      <c r="AE41" s="170"/>
-      <c r="AF41" s="170"/>
-      <c r="AG41" s="170"/>
-      <c r="AH41" s="170"/>
-      <c r="AI41" s="170"/>
-      <c r="AJ41" s="170"/>
-      <c r="AK41" s="171"/>
+      <c r="B41" s="172"/>
+      <c r="C41" s="172"/>
+      <c r="D41" s="172"/>
+      <c r="E41" s="172"/>
+      <c r="F41" s="172"/>
+      <c r="G41" s="172"/>
+      <c r="H41" s="172"/>
+      <c r="I41" s="172"/>
+      <c r="J41" s="172"/>
+      <c r="K41" s="172"/>
+      <c r="L41" s="172"/>
+      <c r="M41" s="172"/>
+      <c r="N41" s="172"/>
+      <c r="O41" s="172"/>
+      <c r="P41" s="172"/>
+      <c r="Q41" s="172"/>
+      <c r="R41" s="172"/>
+      <c r="S41" s="172"/>
+      <c r="T41" s="172"/>
+      <c r="U41" s="172"/>
+      <c r="V41" s="172"/>
+      <c r="W41" s="172"/>
+      <c r="X41" s="172"/>
+      <c r="Y41" s="172"/>
+      <c r="Z41" s="172"/>
+      <c r="AA41" s="172"/>
+      <c r="AB41" s="172"/>
+      <c r="AC41" s="172"/>
+      <c r="AD41" s="172"/>
+      <c r="AE41" s="172"/>
+      <c r="AF41" s="172"/>
+      <c r="AG41" s="172"/>
+      <c r="AH41" s="172"/>
+      <c r="AI41" s="172"/>
+      <c r="AJ41" s="172"/>
+      <c r="AK41" s="173"/>
     </row>
-    <row r="42" spans="1:41">
-      <c r="A42" s="172" t="s">
-        <v>0</v>
-      </c>
-      <c r="B42" s="170"/>
-      <c r="C42" s="170" t="s">
+    <row r="42" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A42" s="171" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="172"/>
+      <c r="C42" s="172" t="s">
         <v>6</v>
       </c>
-      <c r="D42" s="170"/>
-      <c r="E42" s="170"/>
-      <c r="F42" s="170"/>
-      <c r="G42" s="170"/>
-      <c r="H42" s="170"/>
-      <c r="I42" s="170"/>
-      <c r="J42" s="170"/>
-      <c r="K42" s="170"/>
-      <c r="L42" s="170"/>
-      <c r="M42" s="170"/>
-      <c r="N42" s="170"/>
-      <c r="O42" s="170"/>
-      <c r="P42" s="170"/>
-      <c r="Q42" s="170"/>
-      <c r="R42" s="171"/>
+      <c r="D42" s="172"/>
+      <c r="E42" s="172"/>
+      <c r="F42" s="172"/>
+      <c r="G42" s="172"/>
+      <c r="H42" s="172"/>
+      <c r="I42" s="172"/>
+      <c r="J42" s="172"/>
+      <c r="K42" s="172"/>
+      <c r="L42" s="172"/>
+      <c r="M42" s="172"/>
+      <c r="N42" s="172"/>
+      <c r="O42" s="172"/>
+      <c r="P42" s="172"/>
+      <c r="Q42" s="172"/>
+      <c r="R42" s="173"/>
       <c r="S42" s="124" t="s">
         <v>141</v>
       </c>
-      <c r="T42" s="172" t="s">
+      <c r="T42" s="171" t="s">
         <v>109</v>
       </c>
-      <c r="U42" s="170"/>
-      <c r="V42" s="170" t="s">
+      <c r="U42" s="172"/>
+      <c r="V42" s="172" t="s">
         <v>12</v>
       </c>
-      <c r="W42" s="170"/>
-      <c r="X42" s="170"/>
-      <c r="Y42" s="170"/>
-      <c r="Z42" s="170"/>
-      <c r="AA42" s="170"/>
-      <c r="AB42" s="170"/>
-      <c r="AC42" s="170"/>
-      <c r="AD42" s="170"/>
-      <c r="AE42" s="170"/>
-      <c r="AF42" s="170"/>
-      <c r="AG42" s="170"/>
-      <c r="AH42" s="170"/>
-      <c r="AI42" s="170"/>
-      <c r="AJ42" s="170"/>
-      <c r="AK42" s="171"/>
+      <c r="W42" s="172"/>
+      <c r="X42" s="172"/>
+      <c r="Y42" s="172"/>
+      <c r="Z42" s="172"/>
+      <c r="AA42" s="172"/>
+      <c r="AB42" s="172"/>
+      <c r="AC42" s="172"/>
+      <c r="AD42" s="172"/>
+      <c r="AE42" s="172"/>
+      <c r="AF42" s="172"/>
+      <c r="AG42" s="172"/>
+      <c r="AH42" s="172"/>
+      <c r="AI42" s="172"/>
+      <c r="AJ42" s="172"/>
+      <c r="AK42" s="173"/>
     </row>
-    <row r="43" spans="1:41" ht="15.75" thickBot="1">
-      <c r="A43" s="173"/>
-      <c r="B43" s="174"/>
+    <row r="43" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="174"/>
+      <c r="B43" s="176"/>
       <c r="C43" s="10">
         <f>C$15</f>
         <v>0</v>
@@ -11024,8 +11180,8 @@
         <v>140</v>
       </c>
       <c r="S43" s="125"/>
-      <c r="T43" s="173"/>
-      <c r="U43" s="174"/>
+      <c r="T43" s="174"/>
+      <c r="U43" s="176"/>
       <c r="V43" s="10">
         <f t="shared" ref="V43:AK43" si="7">C15</f>
         <v>0</v>
@@ -11091,8 +11247,8 @@
         <v>140</v>
       </c>
     </row>
-    <row r="44" spans="1:41">
-      <c r="A44" s="173" t="s">
+    <row r="44" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A44" s="174" t="s">
         <v>108</v>
       </c>
       <c r="B44" s="83">
@@ -11164,7 +11320,7 @@
         <v>59.074360761700326</v>
       </c>
       <c r="S44" s="125"/>
-      <c r="T44" s="173" t="s">
+      <c r="T44" s="174" t="s">
         <v>5</v>
       </c>
       <c r="U44" s="10">
@@ -11236,8 +11392,8 @@
         <v>1119.7341676529832</v>
       </c>
     </row>
-    <row r="45" spans="1:41">
-      <c r="A45" s="173"/>
+    <row r="45" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A45" s="174"/>
       <c r="B45" s="83">
         <f t="shared" si="8"/>
         <v>20.741350724754323</v>
@@ -11307,7 +11463,7 @@
         <v>61.932797572750339</v>
       </c>
       <c r="S45" s="125"/>
-      <c r="T45" s="173"/>
+      <c r="T45" s="174"/>
       <c r="U45" s="10">
         <f t="shared" si="10"/>
         <v>650</v>
@@ -11377,8 +11533,8 @@
         <v>1119.7341676529829</v>
       </c>
     </row>
-    <row r="46" spans="1:41">
-      <c r="A46" s="173"/>
+    <row r="46" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A46" s="174"/>
       <c r="B46" s="83">
         <f t="shared" si="8"/>
         <v>25.527816276620705</v>
@@ -11448,7 +11604,7 @@
         <v>76.224981628000421</v>
       </c>
       <c r="S46" s="125"/>
-      <c r="T46" s="173"/>
+      <c r="T46" s="174"/>
       <c r="U46" s="10">
         <f t="shared" si="10"/>
         <v>800</v>
@@ -11521,9 +11677,11 @@
       <c r="AM46" s="2"/>
       <c r="AN46" s="2"/>
       <c r="AO46" s="2"/>
+      <c r="AP46" s="2"/>
+      <c r="AQ46" s="2"/>
     </row>
-    <row r="47" spans="1:41">
-      <c r="A47" s="173"/>
+    <row r="47" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A47" s="174"/>
       <c r="B47" s="83">
         <f t="shared" si="8"/>
         <v>31.909770345775883</v>
@@ -11593,7 +11751,7 @@
         <v>95.281227035000555</v>
       </c>
       <c r="S47" s="125"/>
-      <c r="T47" s="173"/>
+      <c r="T47" s="174"/>
       <c r="U47" s="10">
         <f t="shared" si="10"/>
         <v>1000</v>
@@ -11666,9 +11824,11 @@
       <c r="AM47" s="2"/>
       <c r="AN47" s="2"/>
       <c r="AO47" s="2"/>
+      <c r="AP47" s="2"/>
+      <c r="AQ47" s="2"/>
     </row>
-    <row r="48" spans="1:41">
-      <c r="A48" s="173"/>
+    <row r="48" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A48" s="174"/>
       <c r="B48" s="83">
         <f t="shared" si="8"/>
         <v>38.29172441493106</v>
@@ -11738,7 +11898,7 @@
         <v>114.33747244200066</v>
       </c>
       <c r="S48" s="125"/>
-      <c r="T48" s="173"/>
+      <c r="T48" s="174"/>
       <c r="U48" s="10">
         <f t="shared" si="10"/>
         <v>1200</v>
@@ -11811,9 +11971,11 @@
       <c r="AM48" s="2"/>
       <c r="AN48" s="2"/>
       <c r="AO48" s="2"/>
+      <c r="AP48" s="2"/>
+      <c r="AQ48" s="2"/>
     </row>
-    <row r="49" spans="1:41">
-      <c r="A49" s="173"/>
+    <row r="49" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A49" s="174"/>
       <c r="B49" s="83">
         <f t="shared" si="8"/>
         <v>44.673678484086231</v>
@@ -11883,7 +12045,7 @@
         <v>133.39371784900075</v>
       </c>
       <c r="S49" s="125"/>
-      <c r="T49" s="173"/>
+      <c r="T49" s="174"/>
       <c r="U49" s="10">
         <f t="shared" si="10"/>
         <v>1400</v>
@@ -11956,9 +12118,11 @@
       <c r="AM49" s="2"/>
       <c r="AN49" s="2"/>
       <c r="AO49" s="2"/>
+      <c r="AP49" s="2"/>
+      <c r="AQ49" s="2"/>
     </row>
-    <row r="50" spans="1:41">
-      <c r="A50" s="173"/>
+    <row r="50" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A50" s="174"/>
       <c r="B50" s="83">
         <f t="shared" si="8"/>
         <v>49.460144035952617</v>
@@ -12028,7 +12192,7 @@
         <v>147.68590190425081</v>
       </c>
       <c r="S50" s="125"/>
-      <c r="T50" s="173"/>
+      <c r="T50" s="174"/>
       <c r="U50" s="10">
         <f t="shared" si="10"/>
         <v>1550</v>
@@ -12101,9 +12265,11 @@
       <c r="AM50" s="2"/>
       <c r="AN50" s="2"/>
       <c r="AO50" s="2"/>
+      <c r="AP50" s="2"/>
+      <c r="AQ50" s="2"/>
     </row>
-    <row r="51" spans="1:41">
-      <c r="A51" s="173"/>
+    <row r="51" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A51" s="174"/>
       <c r="B51" s="83">
         <f t="shared" si="8"/>
         <v>54.246609587819002</v>
@@ -12173,7 +12339,7 @@
         <v>161.97808595950096</v>
       </c>
       <c r="S51" s="125"/>
-      <c r="T51" s="173"/>
+      <c r="T51" s="174"/>
       <c r="U51" s="10">
         <f t="shared" si="10"/>
         <v>1700</v>
@@ -12246,9 +12412,11 @@
       <c r="AM51" s="2"/>
       <c r="AN51" s="2"/>
       <c r="AO51" s="2"/>
+      <c r="AP51" s="2"/>
+      <c r="AQ51" s="2"/>
     </row>
-    <row r="52" spans="1:41">
-      <c r="A52" s="173"/>
+    <row r="52" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A52" s="174"/>
       <c r="B52" s="83">
         <f t="shared" si="8"/>
         <v>57.437586622396587</v>
@@ -12318,7 +12486,7 @@
         <v>171.50620866300099</v>
       </c>
       <c r="S52" s="125"/>
-      <c r="T52" s="173"/>
+      <c r="T52" s="174"/>
       <c r="U52" s="10">
         <f t="shared" si="10"/>
         <v>1800</v>
@@ -12391,9 +12559,11 @@
       <c r="AM52" s="2"/>
       <c r="AN52" s="2"/>
       <c r="AO52" s="2"/>
+      <c r="AP52" s="2"/>
+      <c r="AQ52" s="2"/>
     </row>
-    <row r="53" spans="1:41">
-      <c r="A53" s="173"/>
+    <row r="53" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A53" s="174"/>
       <c r="B53" s="83">
         <f t="shared" si="8"/>
         <v>63.819540691551765</v>
@@ -12463,7 +12633,7 @@
         <v>190.56245407000111</v>
       </c>
       <c r="S53" s="125"/>
-      <c r="T53" s="173"/>
+      <c r="T53" s="174"/>
       <c r="U53" s="10">
         <f t="shared" si="10"/>
         <v>2000</v>
@@ -12536,9 +12706,11 @@
       <c r="AM53" s="2"/>
       <c r="AN53" s="2"/>
       <c r="AO53" s="2"/>
+      <c r="AP53" s="2"/>
+      <c r="AQ53" s="2"/>
     </row>
-    <row r="54" spans="1:41">
-      <c r="A54" s="173"/>
+    <row r="54" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A54" s="174"/>
       <c r="B54" s="83">
         <f t="shared" si="8"/>
         <v>70.201494760706936</v>
@@ -12608,7 +12780,7 @@
         <v>209.61869947700117</v>
       </c>
       <c r="S54" s="125"/>
-      <c r="T54" s="173"/>
+      <c r="T54" s="174"/>
       <c r="U54" s="10">
         <f t="shared" si="10"/>
         <v>2200</v>
@@ -12681,9 +12853,11 @@
       <c r="AM54" s="2"/>
       <c r="AN54" s="2"/>
       <c r="AO54" s="2"/>
+      <c r="AP54" s="2"/>
+      <c r="AQ54" s="2"/>
     </row>
-    <row r="55" spans="1:41">
-      <c r="A55" s="173"/>
+    <row r="55" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A55" s="174"/>
       <c r="B55" s="83">
         <f t="shared" si="8"/>
         <v>76.583448829862121</v>
@@ -12753,7 +12927,7 @@
         <v>228.67494488400132</v>
       </c>
       <c r="S55" s="125"/>
-      <c r="T55" s="173"/>
+      <c r="T55" s="174"/>
       <c r="U55" s="10">
         <f t="shared" si="10"/>
         <v>2400</v>
@@ -12826,9 +13000,11 @@
       <c r="AM55" s="2"/>
       <c r="AN55" s="2"/>
       <c r="AO55" s="2"/>
+      <c r="AP55" s="2"/>
+      <c r="AQ55" s="2"/>
     </row>
-    <row r="56" spans="1:41">
-      <c r="A56" s="173"/>
+    <row r="56" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A56" s="174"/>
       <c r="B56" s="83">
         <f t="shared" si="8"/>
         <v>82.965402899017292</v>
@@ -12898,7 +13074,7 @@
         <v>247.73119029100135</v>
       </c>
       <c r="S56" s="125"/>
-      <c r="T56" s="173"/>
+      <c r="T56" s="174"/>
       <c r="U56" s="10">
         <f t="shared" si="10"/>
         <v>2600</v>
@@ -12971,9 +13147,11 @@
       <c r="AM56" s="2"/>
       <c r="AN56" s="2"/>
       <c r="AO56" s="2"/>
+      <c r="AP56" s="2"/>
+      <c r="AQ56" s="2"/>
     </row>
-    <row r="57" spans="1:41">
-      <c r="A57" s="173"/>
+    <row r="57" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A57" s="174"/>
       <c r="B57" s="83">
         <f t="shared" si="8"/>
         <v>89.347356968172463</v>
@@ -13043,7 +13221,7 @@
         <v>266.7874356980015</v>
       </c>
       <c r="S57" s="125"/>
-      <c r="T57" s="173"/>
+      <c r="T57" s="174"/>
       <c r="U57" s="10">
         <f t="shared" si="10"/>
         <v>2800</v>
@@ -13116,9 +13294,11 @@
       <c r="AM57" s="2"/>
       <c r="AN57" s="2"/>
       <c r="AO57" s="2"/>
+      <c r="AP57" s="2"/>
+      <c r="AQ57" s="2"/>
     </row>
-    <row r="58" spans="1:41">
-      <c r="A58" s="173"/>
+    <row r="58" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A58" s="174"/>
       <c r="B58" s="83">
         <f t="shared" si="8"/>
         <v>92.538334002750062</v>
@@ -13190,7 +13370,7 @@
       <c r="S58" s="125" t="s">
         <v>140</v>
       </c>
-      <c r="T58" s="173"/>
+      <c r="T58" s="174"/>
       <c r="U58" s="10">
         <f t="shared" si="10"/>
         <v>2900</v>
@@ -13263,9 +13443,11 @@
       <c r="AM58" s="2"/>
       <c r="AN58" s="2"/>
       <c r="AO58" s="2"/>
+      <c r="AP58" s="2"/>
+      <c r="AQ58" s="2"/>
     </row>
-    <row r="59" spans="1:41">
-      <c r="A59" s="173"/>
+    <row r="59" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A59" s="174"/>
       <c r="B59" s="83">
         <f t="shared" si="8"/>
         <v>95.729311037327648</v>
@@ -13335,7 +13517,7 @@
         <v>285.84368110500162</v>
       </c>
       <c r="S59" s="125"/>
-      <c r="T59" s="173"/>
+      <c r="T59" s="174"/>
       <c r="U59" s="10">
         <f t="shared" si="10"/>
         <v>3000</v>
@@ -13408,9 +13590,11 @@
       <c r="AM59" s="2"/>
       <c r="AN59" s="2"/>
       <c r="AO59" s="2"/>
+      <c r="AP59" s="2"/>
+      <c r="AQ59" s="2"/>
     </row>
-    <row r="60" spans="1:41">
-      <c r="A60" s="173"/>
+    <row r="60" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A60" s="174"/>
       <c r="B60" s="83">
         <f t="shared" si="8"/>
         <v>102.11126510648282</v>
@@ -13480,7 +13664,7 @@
         <v>304.89992651200168</v>
       </c>
       <c r="S60" s="125"/>
-      <c r="T60" s="173"/>
+      <c r="T60" s="174"/>
       <c r="U60" s="10">
         <f t="shared" si="10"/>
         <v>3200</v>
@@ -13553,9 +13737,11 @@
       <c r="AM60" s="2"/>
       <c r="AN60" s="2"/>
       <c r="AO60" s="2"/>
+      <c r="AP60" s="2"/>
+      <c r="AQ60" s="2"/>
     </row>
-    <row r="61" spans="1:41">
-      <c r="A61" s="173"/>
+    <row r="61" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A61" s="174"/>
       <c r="B61" s="83">
         <f t="shared" si="8"/>
         <v>105.30224214106042</v>
@@ -13625,7 +13811,7 @@
         <v>314.4280492155018</v>
       </c>
       <c r="S61" s="125"/>
-      <c r="T61" s="173"/>
+      <c r="T61" s="174"/>
       <c r="U61" s="10">
         <f t="shared" si="10"/>
         <v>3300</v>
@@ -13698,9 +13884,11 @@
       <c r="AM61" s="2"/>
       <c r="AN61" s="2"/>
       <c r="AO61" s="2"/>
+      <c r="AP61" s="2"/>
+      <c r="AQ61" s="2"/>
     </row>
-    <row r="62" spans="1:41">
-      <c r="A62" s="173"/>
+    <row r="62" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A62" s="174"/>
       <c r="B62" s="83">
         <f t="shared" si="8"/>
         <v>111.68419621021559</v>
@@ -13772,7 +13960,7 @@
       <c r="S62" s="125" t="s">
         <v>4</v>
       </c>
-      <c r="T62" s="173"/>
+      <c r="T62" s="174"/>
       <c r="U62" s="10">
         <f t="shared" si="10"/>
         <v>3500</v>
@@ -13845,12 +14033,14 @@
       <c r="AM62" s="2"/>
       <c r="AN62" s="2"/>
       <c r="AO62" s="2"/>
+      <c r="AP62" s="2"/>
+      <c r="AQ62" s="2"/>
     </row>
-    <row r="63" spans="1:41">
-      <c r="A63" s="173"/>
+    <row r="63" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A63" s="174"/>
       <c r="B63" s="83">
         <f t="shared" si="8"/>
-        <v>127.63908138310353</v>
+        <v>121.25712731394835</v>
       </c>
       <c r="C63" s="71">
         <f t="shared" si="12"/>
@@ -13858,69 +14048,69 @@
       </c>
       <c r="D63" s="64">
         <f t="shared" si="13"/>
-        <v>27.223207724285874</v>
+        <v>25.862047338071566</v>
       </c>
       <c r="E63" s="64">
         <f t="shared" si="14"/>
-        <v>54.446415448571749</v>
+        <v>51.724094676143132</v>
       </c>
       <c r="F63" s="64">
         <f t="shared" si="15"/>
-        <v>81.669623172857598</v>
+        <v>77.586142014214715</v>
       </c>
       <c r="G63" s="64">
         <f t="shared" si="16"/>
-        <v>122.50443475928643</v>
+        <v>116.3792130213221</v>
       </c>
       <c r="H63" s="64">
         <f t="shared" si="17"/>
-        <v>149.72764248357225</v>
+        <v>142.24126035939361</v>
       </c>
       <c r="I63" s="64">
         <f t="shared" si="18"/>
-        <v>176.95085020785805</v>
+        <v>168.10330769746523</v>
       </c>
       <c r="J63" s="64">
         <f t="shared" si="19"/>
-        <v>204.17405793214397</v>
+        <v>193.96535503553673</v>
       </c>
       <c r="K63" s="64">
         <f t="shared" si="20"/>
-        <v>231.39726565642985</v>
+        <v>219.82740237360835</v>
       </c>
       <c r="L63" s="64">
         <f t="shared" si="21"/>
-        <v>258.62047338071574</v>
+        <v>245.68944971168</v>
       </c>
       <c r="M63" s="64">
         <f t="shared" si="22"/>
-        <v>299.45528496714451</v>
+        <v>284.48252071878721</v>
       </c>
       <c r="N63" s="64">
         <f t="shared" si="23"/>
-        <v>326.67849269143039</v>
+        <v>310.34456805685886</v>
       </c>
       <c r="O63" s="64">
         <f t="shared" si="24"/>
-        <v>340.29009655357339</v>
+        <v>323.27559172589463</v>
       </c>
       <c r="P63" s="64">
         <f t="shared" si="25"/>
-        <v>353.90170041571611</v>
+        <v>336.20661539493045</v>
       </c>
       <c r="Q63" s="64">
         <f t="shared" si="26"/>
-        <v>367.51330427785899</v>
+        <v>349.13763906396622</v>
       </c>
       <c r="R63" s="65">
         <f t="shared" si="27"/>
-        <v>381.12490814000222</v>
+        <v>362.06866273300204</v>
       </c>
       <c r="S63" s="125"/>
-      <c r="T63" s="173"/>
+      <c r="T63" s="174"/>
       <c r="U63" s="10">
         <f t="shared" si="10"/>
-        <v>4000</v>
+        <v>3800</v>
       </c>
       <c r="V63" s="71">
         <f t="shared" ref="V63:AK63" si="46">((V35*$B$39)/(Tire_Wheel_Radius/12))*(Drivetrain_Efficiency/100)</f>
@@ -13928,15 +14118,15 @@
       </c>
       <c r="W63" s="64">
         <f t="shared" si="46"/>
-        <v>79.981011975213107</v>
+        <v>79.981011975213065</v>
       </c>
       <c r="X63" s="64">
         <f t="shared" si="46"/>
-        <v>159.96202395042621</v>
+        <v>159.96202395042613</v>
       </c>
       <c r="Y63" s="64">
         <f t="shared" si="46"/>
-        <v>239.94303592563921</v>
+        <v>239.94303592563924</v>
       </c>
       <c r="Z63" s="64">
         <f t="shared" si="46"/>
@@ -13948,11 +14138,11 @@
       </c>
       <c r="AB63" s="64">
         <f t="shared" si="46"/>
-        <v>519.87657783888483</v>
+        <v>519.87657783888505</v>
       </c>
       <c r="AC63" s="64">
         <f t="shared" si="46"/>
-        <v>599.85758981409799</v>
+        <v>599.85758981409788</v>
       </c>
       <c r="AD63" s="64">
         <f t="shared" si="46"/>
@@ -13960,7 +14150,7 @@
       </c>
       <c r="AE63" s="64">
         <f t="shared" si="46"/>
-        <v>759.81961376452421</v>
+        <v>759.81961376452443</v>
       </c>
       <c r="AF63" s="64">
         <f t="shared" si="46"/>
@@ -13968,30 +14158,32 @@
       </c>
       <c r="AG63" s="64">
         <f t="shared" si="46"/>
-        <v>959.77214370255683</v>
+        <v>959.77214370255695</v>
       </c>
       <c r="AH63" s="64">
         <f t="shared" si="46"/>
-        <v>999.76264969016358</v>
+        <v>999.76264969016347</v>
       </c>
       <c r="AI63" s="64">
         <f t="shared" si="46"/>
-        <v>1039.7531556777697</v>
+        <v>1039.7531556777701</v>
       </c>
       <c r="AJ63" s="64">
         <f t="shared" si="46"/>
-        <v>1079.7436616653761</v>
+        <v>1079.7436616653765</v>
       </c>
       <c r="AK63" s="65">
         <f t="shared" si="46"/>
-        <v>1119.7341676529834</v>
+        <v>1119.7341676529832</v>
       </c>
       <c r="AL63" s="2"/>
       <c r="AM63" s="2"/>
       <c r="AN63" s="2"/>
       <c r="AO63" s="2"/>
+      <c r="AP63" s="2"/>
+      <c r="AQ63" s="2"/>
     </row>
-    <row r="64" spans="1:41" ht="15.75" thickBot="1">
+    <row r="64" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="175"/>
       <c r="B64" s="84">
         <f t="shared" si="8"/>
@@ -14135,8 +14327,10 @@
       <c r="AM64" s="2"/>
       <c r="AN64" s="2"/>
       <c r="AO64" s="2"/>
+      <c r="AP64" s="2"/>
+      <c r="AQ64" s="2"/>
     </row>
-    <row r="65" spans="3:41">
+    <row r="65" spans="3:43" x14ac:dyDescent="0.25">
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
@@ -14169,8 +14363,10 @@
       <c r="AM65" s="2"/>
       <c r="AN65" s="2"/>
       <c r="AO65" s="2"/>
+      <c r="AP65" s="2"/>
+      <c r="AQ65" s="2"/>
     </row>
-    <row r="66" spans="3:41">
+    <row r="66" spans="3:43" x14ac:dyDescent="0.25">
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
@@ -14203,8 +14399,10 @@
       <c r="AM66" s="2"/>
       <c r="AN66" s="2"/>
       <c r="AO66" s="2"/>
+      <c r="AP66" s="2"/>
+      <c r="AQ66" s="2"/>
     </row>
-    <row r="67" spans="3:41">
+    <row r="67" spans="3:43" x14ac:dyDescent="0.25">
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
@@ -14223,17 +14421,18 @@
       <c r="R67" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection password="CC3D" sheet="1" objects="1" scenarios="1" formatColumns="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="ycXf1EGxSd3tVRSHWJQLPZJIMDnRHVFV4ye1dtiwpsJZwFpyjRoXFDGWRXv8ehHXsVqbo4o/bzbp0cyS7jXZvQ==" saltValue="+BAHdaIiBUNp1gwBk+Z4nQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatColumns="0"/>
   <dataConsolidate/>
-  <mergeCells count="21">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A41:AK41"/>
+  <mergeCells count="22">
+    <mergeCell ref="AP14:AW14"/>
+    <mergeCell ref="C14:R14"/>
+    <mergeCell ref="A14:B15"/>
+    <mergeCell ref="A16:A36"/>
+    <mergeCell ref="T14:U15"/>
+    <mergeCell ref="AP18:AR18"/>
+    <mergeCell ref="AL14:AL36"/>
     <mergeCell ref="A44:A64"/>
     <mergeCell ref="T44:T64"/>
-    <mergeCell ref="A13:AK13"/>
     <mergeCell ref="A42:B43"/>
     <mergeCell ref="C42:R42"/>
     <mergeCell ref="T42:U43"/>
@@ -14241,31 +14440,31 @@
     <mergeCell ref="V14:AK14"/>
     <mergeCell ref="T16:T36"/>
     <mergeCell ref="A38:B38"/>
-    <mergeCell ref="AN14:AU14"/>
-    <mergeCell ref="C14:R14"/>
-    <mergeCell ref="A14:B15"/>
-    <mergeCell ref="A16:A36"/>
-    <mergeCell ref="T14:U15"/>
-    <mergeCell ref="AN18:AP18"/>
+    <mergeCell ref="A13:AM13"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A41:AK41"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:R36">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V16:AK36">
+  <conditionalFormatting sqref="AM16:AM36 V16:AK36">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -14275,9 +14474,9 @@
   <conditionalFormatting sqref="C44:R64">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -14287,30 +14486,31 @@
   <conditionalFormatting sqref="V44:AK64">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Gear" prompt="Select the gear to view." sqref="A38:B38">
-      <formula1>Gear!G4:Z4</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <extLst xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
+  <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4DAE18C3-50A6-4B4C-A87A-971841D29C1E}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Gear!$G$4:$Z$4</xm:f>
           </x14:formula1>
           <xm:sqref>A38</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Gear" prompt="Select the gear to view.">
+          <x14:formula1>
+            <xm:f>Gear!G4:Z4</xm:f>
+          </x14:formula1>
+          <xm:sqref>A38:B38</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -14319,14 +14519,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ48"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.28515625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="13.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
@@ -14346,99 +14546,99 @@
     <col min="44" max="16384" width="13.28515625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="15.75" thickBot="1">
-      <c r="A1" s="181" t="s">
+    <row r="1" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="180" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="182"/>
-      <c r="C1" s="182"/>
-      <c r="D1" s="182"/>
-      <c r="E1" s="182"/>
-      <c r="F1" s="182"/>
-      <c r="G1" s="182"/>
-      <c r="H1" s="182"/>
-      <c r="I1" s="182"/>
-      <c r="J1" s="182"/>
-      <c r="K1" s="182"/>
-      <c r="L1" s="182"/>
-      <c r="M1" s="182"/>
-      <c r="N1" s="182"/>
-      <c r="O1" s="182"/>
-      <c r="P1" s="182"/>
-      <c r="Q1" s="182"/>
-      <c r="R1" s="182"/>
-      <c r="S1" s="182"/>
-      <c r="T1" s="182"/>
-      <c r="U1" s="182"/>
-      <c r="V1" s="182"/>
-      <c r="W1" s="182"/>
-      <c r="X1" s="182"/>
-      <c r="Y1" s="182"/>
-      <c r="Z1" s="182"/>
-      <c r="AA1" s="182"/>
-      <c r="AB1" s="182"/>
-      <c r="AC1" s="182"/>
-      <c r="AD1" s="182"/>
-      <c r="AE1" s="182"/>
-      <c r="AF1" s="182"/>
-      <c r="AG1" s="182"/>
-      <c r="AH1" s="182"/>
-      <c r="AI1" s="182"/>
-      <c r="AJ1" s="182"/>
-      <c r="AK1" s="183"/>
+      <c r="B1" s="181"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="181"/>
+      <c r="E1" s="181"/>
+      <c r="F1" s="181"/>
+      <c r="G1" s="181"/>
+      <c r="H1" s="181"/>
+      <c r="I1" s="181"/>
+      <c r="J1" s="181"/>
+      <c r="K1" s="181"/>
+      <c r="L1" s="181"/>
+      <c r="M1" s="181"/>
+      <c r="N1" s="181"/>
+      <c r="O1" s="181"/>
+      <c r="P1" s="181"/>
+      <c r="Q1" s="181"/>
+      <c r="R1" s="181"/>
+      <c r="S1" s="181"/>
+      <c r="T1" s="181"/>
+      <c r="U1" s="181"/>
+      <c r="V1" s="181"/>
+      <c r="W1" s="181"/>
+      <c r="X1" s="181"/>
+      <c r="Y1" s="181"/>
+      <c r="Z1" s="181"/>
+      <c r="AA1" s="181"/>
+      <c r="AB1" s="181"/>
+      <c r="AC1" s="181"/>
+      <c r="AD1" s="181"/>
+      <c r="AE1" s="181"/>
+      <c r="AF1" s="181"/>
+      <c r="AG1" s="181"/>
+      <c r="AH1" s="181"/>
+      <c r="AI1" s="181"/>
+      <c r="AJ1" s="181"/>
+      <c r="AK1" s="182"/>
     </row>
-    <row r="2" spans="1:37">
-      <c r="A2" s="172" t="s">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A2" s="171" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="170"/>
-      <c r="C2" s="170" t="s">
+      <c r="B2" s="172"/>
+      <c r="C2" s="172" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
-      <c r="I2" s="170"/>
-      <c r="J2" s="170"/>
-      <c r="K2" s="170"/>
-      <c r="L2" s="170"/>
-      <c r="M2" s="170"/>
-      <c r="N2" s="170"/>
-      <c r="O2" s="170"/>
-      <c r="P2" s="170"/>
-      <c r="Q2" s="170"/>
-      <c r="R2" s="171"/>
+      <c r="D2" s="172"/>
+      <c r="E2" s="172"/>
+      <c r="F2" s="172"/>
+      <c r="G2" s="172"/>
+      <c r="H2" s="172"/>
+      <c r="I2" s="172"/>
+      <c r="J2" s="172"/>
+      <c r="K2" s="172"/>
+      <c r="L2" s="172"/>
+      <c r="M2" s="172"/>
+      <c r="N2" s="172"/>
+      <c r="O2" s="172"/>
+      <c r="P2" s="172"/>
+      <c r="Q2" s="172"/>
+      <c r="R2" s="173"/>
       <c r="S2" s="121" t="s">
         <v>141</v>
       </c>
-      <c r="T2" s="172" t="s">
+      <c r="T2" s="171" t="s">
         <v>3</v>
       </c>
-      <c r="U2" s="170"/>
-      <c r="V2" s="170" t="s">
+      <c r="U2" s="172"/>
+      <c r="V2" s="172" t="s">
         <v>12</v>
       </c>
-      <c r="W2" s="170"/>
-      <c r="X2" s="170"/>
-      <c r="Y2" s="170"/>
-      <c r="Z2" s="170"/>
-      <c r="AA2" s="170"/>
-      <c r="AB2" s="170"/>
-      <c r="AC2" s="170"/>
-      <c r="AD2" s="170"/>
-      <c r="AE2" s="170"/>
-      <c r="AF2" s="170"/>
-      <c r="AG2" s="170"/>
-      <c r="AH2" s="170"/>
-      <c r="AI2" s="170"/>
-      <c r="AJ2" s="170"/>
-      <c r="AK2" s="171"/>
+      <c r="W2" s="172"/>
+      <c r="X2" s="172"/>
+      <c r="Y2" s="172"/>
+      <c r="Z2" s="172"/>
+      <c r="AA2" s="172"/>
+      <c r="AB2" s="172"/>
+      <c r="AC2" s="172"/>
+      <c r="AD2" s="172"/>
+      <c r="AE2" s="172"/>
+      <c r="AF2" s="172"/>
+      <c r="AG2" s="172"/>
+      <c r="AH2" s="172"/>
+      <c r="AI2" s="172"/>
+      <c r="AJ2" s="172"/>
+      <c r="AK2" s="173"/>
     </row>
-    <row r="3" spans="1:37" ht="15.75" thickBot="1">
-      <c r="A3" s="173"/>
-      <c r="B3" s="174"/>
+    <row r="3" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="174"/>
+      <c r="B3" s="176"/>
       <c r="C3" s="107">
         <v>0</v>
       </c>
@@ -14488,8 +14688,8 @@
         <v>140</v>
       </c>
       <c r="S3" s="127"/>
-      <c r="T3" s="173"/>
-      <c r="U3" s="174"/>
+      <c r="T3" s="174"/>
+      <c r="U3" s="176"/>
       <c r="V3" s="74">
         <f t="shared" ref="V3:AK3" si="0">C3</f>
         <v>0</v>
@@ -14555,8 +14755,8 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
-      <c r="A4" s="173" t="s">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A4" s="174" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="107">
@@ -14611,7 +14811,7 @@
         <v>4.2798910000000001</v>
       </c>
       <c r="S4" s="127"/>
-      <c r="T4" s="173" t="s">
+      <c r="T4" s="174" t="s">
         <v>5</v>
       </c>
       <c r="U4" s="74">
@@ -14667,8 +14867,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:37">
-      <c r="A5" s="173"/>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A5" s="174"/>
       <c r="B5" s="111">
         <v>650</v>
       </c>
@@ -14721,7 +14921,7 @@
         <v>4.2798910000000001</v>
       </c>
       <c r="S5" s="127"/>
-      <c r="T5" s="173"/>
+      <c r="T5" s="174"/>
       <c r="U5" s="74">
         <f t="shared" si="1"/>
         <v>650</v>
@@ -14775,8 +14975,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:37">
-      <c r="A6" s="173"/>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A6" s="174"/>
       <c r="B6" s="111">
         <v>800</v>
       </c>
@@ -14829,7 +15029,7 @@
         <v>3.6684779999999999</v>
       </c>
       <c r="S6" s="127"/>
-      <c r="T6" s="173"/>
+      <c r="T6" s="174"/>
       <c r="U6" s="74">
         <f t="shared" si="1"/>
         <v>800</v>
@@ -14883,8 +15083,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
-      <c r="A7" s="173"/>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A7" s="174"/>
       <c r="B7" s="111">
         <v>1000</v>
       </c>
@@ -14937,7 +15137,7 @@
         <v>3.8043480000000001</v>
       </c>
       <c r="S7" s="127"/>
-      <c r="T7" s="173"/>
+      <c r="T7" s="174"/>
       <c r="U7" s="74">
         <f t="shared" si="1"/>
         <v>1000</v>
@@ -14991,8 +15191,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
-      <c r="A8" s="173"/>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A8" s="174"/>
       <c r="B8" s="111">
         <v>1200</v>
       </c>
@@ -15045,7 +15245,7 @@
         <v>5.9782609999999998</v>
       </c>
       <c r="S8" s="127"/>
-      <c r="T8" s="173"/>
+      <c r="T8" s="174"/>
       <c r="U8" s="74">
         <f t="shared" si="1"/>
         <v>1200</v>
@@ -15099,8 +15299,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
-      <c r="A9" s="173"/>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A9" s="174"/>
       <c r="B9" s="111">
         <v>1400</v>
       </c>
@@ -15153,7 +15353,7 @@
         <v>11.684782999999999</v>
       </c>
       <c r="S9" s="127"/>
-      <c r="T9" s="173"/>
+      <c r="T9" s="174"/>
       <c r="U9" s="74">
         <f t="shared" si="1"/>
         <v>1400</v>
@@ -15207,8 +15407,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
-      <c r="A10" s="173"/>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A10" s="174"/>
       <c r="B10" s="111">
         <v>1550</v>
       </c>
@@ -15261,7 +15461,7 @@
         <v>12.975543999999999</v>
       </c>
       <c r="S10" s="127"/>
-      <c r="T10" s="173"/>
+      <c r="T10" s="174"/>
       <c r="U10" s="74">
         <f t="shared" si="1"/>
         <v>1550</v>
@@ -15315,8 +15515,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
-      <c r="A11" s="173"/>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A11" s="174"/>
       <c r="B11" s="111">
         <v>1700</v>
       </c>
@@ -15369,7 +15569,7 @@
         <v>13.994566000000001</v>
       </c>
       <c r="S11" s="127"/>
-      <c r="T11" s="173"/>
+      <c r="T11" s="174"/>
       <c r="U11" s="74">
         <f t="shared" si="1"/>
         <v>1700</v>
@@ -15423,8 +15623,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
-      <c r="A12" s="173"/>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A12" s="174"/>
       <c r="B12" s="111">
         <v>1800</v>
       </c>
@@ -15477,7 +15677,7 @@
         <v>12.975543999999999</v>
       </c>
       <c r="S12" s="127"/>
-      <c r="T12" s="173"/>
+      <c r="T12" s="174"/>
       <c r="U12" s="74">
         <f t="shared" si="1"/>
         <v>1800</v>
@@ -15531,8 +15731,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:37">
-      <c r="A13" s="173"/>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A13" s="174"/>
       <c r="B13" s="111">
         <v>2000</v>
       </c>
@@ -15585,7 +15785,7 @@
         <v>12.975543999999999</v>
       </c>
       <c r="S13" s="127"/>
-      <c r="T13" s="173"/>
+      <c r="T13" s="174"/>
       <c r="U13" s="74">
         <f t="shared" si="1"/>
         <v>2000</v>
@@ -15639,8 +15839,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
-      <c r="A14" s="173"/>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A14" s="174"/>
       <c r="B14" s="111">
         <v>2200</v>
       </c>
@@ -15693,7 +15893,7 @@
         <v>13.315218</v>
       </c>
       <c r="S14" s="127"/>
-      <c r="T14" s="173"/>
+      <c r="T14" s="174"/>
       <c r="U14" s="74">
         <f t="shared" si="1"/>
         <v>2200</v>
@@ -15747,8 +15947,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:37">
-      <c r="A15" s="173"/>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A15" s="174"/>
       <c r="B15" s="111">
         <v>2400</v>
       </c>
@@ -15801,7 +16001,7 @@
         <v>13.111413000000001</v>
       </c>
       <c r="S15" s="127"/>
-      <c r="T15" s="173"/>
+      <c r="T15" s="174"/>
       <c r="U15" s="74">
         <f t="shared" si="1"/>
         <v>2400</v>
@@ -15855,8 +16055,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:37">
-      <c r="A16" s="173"/>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A16" s="174"/>
       <c r="B16" s="111">
         <v>2600</v>
       </c>
@@ -15909,7 +16109,7 @@
         <v>11.480978</v>
       </c>
       <c r="S16" s="127"/>
-      <c r="T16" s="173"/>
+      <c r="T16" s="174"/>
       <c r="U16" s="74">
         <f t="shared" si="1"/>
         <v>2600</v>
@@ -15963,8 +16163,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:43">
-      <c r="A17" s="173"/>
+    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A17" s="174"/>
       <c r="B17" s="111">
         <v>2800</v>
       </c>
@@ -16017,7 +16217,7 @@
         <v>11.005435</v>
       </c>
       <c r="S17" s="127"/>
-      <c r="T17" s="173"/>
+      <c r="T17" s="174"/>
       <c r="U17" s="74">
         <f t="shared" si="1"/>
         <v>2800</v>
@@ -16071,8 +16271,8 @@
         <v>11.073370000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:43">
-      <c r="A18" s="173"/>
+    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A18" s="174"/>
       <c r="B18" s="111">
         <v>2900</v>
       </c>
@@ -16125,7 +16325,7 @@
         <v>9.9864130000000007</v>
       </c>
       <c r="S18" s="127"/>
-      <c r="T18" s="173"/>
+      <c r="T18" s="174"/>
       <c r="U18" s="74">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -16179,8 +16379,8 @@
         <v>12.024457</v>
       </c>
     </row>
-    <row r="19" spans="1:43">
-      <c r="A19" s="173"/>
+    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A19" s="174"/>
       <c r="B19" s="111">
         <v>3000</v>
       </c>
@@ -16233,7 +16433,7 @@
         <v>9.9864130000000007</v>
       </c>
       <c r="S19" s="127"/>
-      <c r="T19" s="173"/>
+      <c r="T19" s="174"/>
       <c r="U19" s="74">
         <f t="shared" si="1"/>
         <v>3000</v>
@@ -16287,8 +16487,8 @@
         <v>11.820652000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:43">
-      <c r="A20" s="173"/>
+    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A20" s="174"/>
       <c r="B20" s="111">
         <v>3200</v>
       </c>
@@ -16341,7 +16541,7 @@
         <v>6.5217390000000002</v>
       </c>
       <c r="S20" s="127"/>
-      <c r="T20" s="173"/>
+      <c r="T20" s="174"/>
       <c r="U20" s="74">
         <f t="shared" si="1"/>
         <v>3200</v>
@@ -16395,8 +16595,8 @@
         <v>11.480978</v>
       </c>
     </row>
-    <row r="21" spans="1:43">
-      <c r="A21" s="173"/>
+    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A21" s="174"/>
       <c r="B21" s="111">
         <v>3300</v>
       </c>
@@ -16449,7 +16649,7 @@
         <v>0</v>
       </c>
       <c r="S21" s="127"/>
-      <c r="T21" s="173"/>
+      <c r="T21" s="174"/>
       <c r="U21" s="74">
         <f t="shared" si="1"/>
         <v>3300</v>
@@ -16503,7 +16703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:43" ht="15.75" thickBot="1">
+    <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="175"/>
       <c r="B22" s="115">
         <v>3500</v>
@@ -16611,14 +16811,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:43" ht="15.75" thickBot="1"/>
-    <row r="24" spans="1:43" ht="15.75" thickBot="1">
-      <c r="A24" s="176" t="s">
+    <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="177" t="s">
         <v>116</v>
       </c>
-      <c r="B24" s="177"/>
+      <c r="B24" s="178"/>
     </row>
-    <row r="25" spans="1:43" ht="15.75" thickBot="1">
+    <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="28" t="s">
         <v>40</v>
       </c>
@@ -16627,7 +16827,7 @@
         <v>2.9467000000000003</v>
       </c>
     </row>
-    <row r="26" spans="1:43" ht="15.75" thickBot="1">
+    <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="28" t="s">
         <v>145</v>
       </c>
@@ -16636,46 +16836,46 @@
         <v>1880.3018432861463</v>
       </c>
     </row>
-    <row r="27" spans="1:43" ht="15.75" thickBot="1">
-      <c r="A27" s="181" t="s">
+    <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="180" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="182"/>
-      <c r="C27" s="182"/>
-      <c r="D27" s="182"/>
-      <c r="E27" s="182"/>
-      <c r="F27" s="182"/>
-      <c r="G27" s="182"/>
-      <c r="H27" s="182"/>
-      <c r="I27" s="182"/>
-      <c r="J27" s="182"/>
-      <c r="K27" s="182"/>
-      <c r="L27" s="182"/>
-      <c r="M27" s="182"/>
-      <c r="N27" s="182"/>
-      <c r="O27" s="182"/>
-      <c r="P27" s="182"/>
-      <c r="Q27" s="182"/>
-      <c r="R27" s="182"/>
-      <c r="S27" s="182"/>
-      <c r="T27" s="182"/>
-      <c r="U27" s="182"/>
-      <c r="V27" s="182"/>
-      <c r="W27" s="182"/>
-      <c r="X27" s="182"/>
-      <c r="Y27" s="182"/>
-      <c r="Z27" s="182"/>
-      <c r="AA27" s="182"/>
-      <c r="AB27" s="182"/>
-      <c r="AC27" s="182"/>
-      <c r="AD27" s="182"/>
-      <c r="AE27" s="182"/>
-      <c r="AF27" s="182"/>
-      <c r="AG27" s="182"/>
-      <c r="AH27" s="182"/>
-      <c r="AI27" s="182"/>
-      <c r="AJ27" s="182"/>
-      <c r="AK27" s="183"/>
+      <c r="B27" s="181"/>
+      <c r="C27" s="181"/>
+      <c r="D27" s="181"/>
+      <c r="E27" s="181"/>
+      <c r="F27" s="181"/>
+      <c r="G27" s="181"/>
+      <c r="H27" s="181"/>
+      <c r="I27" s="181"/>
+      <c r="J27" s="181"/>
+      <c r="K27" s="181"/>
+      <c r="L27" s="181"/>
+      <c r="M27" s="181"/>
+      <c r="N27" s="181"/>
+      <c r="O27" s="181"/>
+      <c r="P27" s="181"/>
+      <c r="Q27" s="181"/>
+      <c r="R27" s="181"/>
+      <c r="S27" s="181"/>
+      <c r="T27" s="181"/>
+      <c r="U27" s="181"/>
+      <c r="V27" s="181"/>
+      <c r="W27" s="181"/>
+      <c r="X27" s="181"/>
+      <c r="Y27" s="181"/>
+      <c r="Z27" s="181"/>
+      <c r="AA27" s="181"/>
+      <c r="AB27" s="181"/>
+      <c r="AC27" s="181"/>
+      <c r="AD27" s="181"/>
+      <c r="AE27" s="181"/>
+      <c r="AF27" s="181"/>
+      <c r="AG27" s="181"/>
+      <c r="AH27" s="181"/>
+      <c r="AI27" s="181"/>
+      <c r="AJ27" s="181"/>
+      <c r="AK27" s="182"/>
       <c r="AM27" s="97" t="s">
         <v>131</v>
       </c>
@@ -16684,65 +16884,65 @@
       <c r="AP27" s="97"/>
       <c r="AQ27" s="97"/>
     </row>
-    <row r="28" spans="1:43">
-      <c r="A28" s="173" t="s">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A28" s="174" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="174"/>
-      <c r="C28" s="174" t="s">
+      <c r="B28" s="176"/>
+      <c r="C28" s="176" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="174"/>
-      <c r="E28" s="174"/>
-      <c r="F28" s="174"/>
-      <c r="G28" s="174"/>
-      <c r="H28" s="174"/>
-      <c r="I28" s="174"/>
-      <c r="J28" s="174"/>
-      <c r="K28" s="174"/>
-      <c r="L28" s="174"/>
-      <c r="M28" s="174"/>
-      <c r="N28" s="174"/>
-      <c r="O28" s="174"/>
-      <c r="P28" s="174"/>
-      <c r="Q28" s="174"/>
-      <c r="R28" s="185"/>
+      <c r="D28" s="176"/>
+      <c r="E28" s="176"/>
+      <c r="F28" s="176"/>
+      <c r="G28" s="176"/>
+      <c r="H28" s="176"/>
+      <c r="I28" s="176"/>
+      <c r="J28" s="176"/>
+      <c r="K28" s="176"/>
+      <c r="L28" s="176"/>
+      <c r="M28" s="176"/>
+      <c r="N28" s="176"/>
+      <c r="O28" s="176"/>
+      <c r="P28" s="176"/>
+      <c r="Q28" s="176"/>
+      <c r="R28" s="184"/>
       <c r="S28" s="124" t="s">
         <v>141</v>
       </c>
-      <c r="T28" s="180" t="s">
+      <c r="T28" s="185" t="s">
         <v>142</v>
       </c>
-      <c r="U28" s="170"/>
-      <c r="V28" s="170" t="s">
+      <c r="U28" s="172"/>
+      <c r="V28" s="172" t="s">
         <v>143</v>
       </c>
-      <c r="W28" s="170"/>
-      <c r="X28" s="170"/>
-      <c r="Y28" s="170"/>
-      <c r="Z28" s="170"/>
-      <c r="AA28" s="170"/>
-      <c r="AB28" s="170"/>
-      <c r="AC28" s="170"/>
-      <c r="AD28" s="170"/>
-      <c r="AE28" s="170"/>
-      <c r="AF28" s="170"/>
-      <c r="AG28" s="170"/>
-      <c r="AH28" s="170"/>
-      <c r="AI28" s="170"/>
-      <c r="AJ28" s="170"/>
-      <c r="AK28" s="171"/>
+      <c r="W28" s="172"/>
+      <c r="X28" s="172"/>
+      <c r="Y28" s="172"/>
+      <c r="Z28" s="172"/>
+      <c r="AA28" s="172"/>
+      <c r="AB28" s="172"/>
+      <c r="AC28" s="172"/>
+      <c r="AD28" s="172"/>
+      <c r="AE28" s="172"/>
+      <c r="AF28" s="172"/>
+      <c r="AG28" s="172"/>
+      <c r="AH28" s="172"/>
+      <c r="AI28" s="172"/>
+      <c r="AJ28" s="172"/>
+      <c r="AK28" s="173"/>
       <c r="AM28" s="97"/>
-      <c r="AN28" s="184" t="s">
+      <c r="AN28" s="183" t="s">
         <v>7</v>
       </c>
-      <c r="AO28" s="184"/>
-      <c r="AP28" s="184"/>
-      <c r="AQ28" s="184"/>
+      <c r="AO28" s="183"/>
+      <c r="AP28" s="183"/>
+      <c r="AQ28" s="183"/>
     </row>
-    <row r="29" spans="1:43" ht="15.75" thickBot="1">
-      <c r="A29" s="173"/>
-      <c r="B29" s="174"/>
+    <row r="29" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="174"/>
+      <c r="B29" s="176"/>
       <c r="C29" s="74">
         <f>C$3</f>
         <v>0</v>
@@ -16808,8 +17008,8 @@
         <v>140</v>
       </c>
       <c r="S29" s="129"/>
-      <c r="T29" s="173"/>
-      <c r="U29" s="174"/>
+      <c r="T29" s="174"/>
+      <c r="U29" s="176"/>
       <c r="V29" s="107">
         <v>1</v>
       </c>
@@ -16874,8 +17074,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:43">
-      <c r="A30" s="173" t="s">
+    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A30" s="174" t="s">
         <v>5</v>
       </c>
       <c r="B30" s="74">
@@ -16947,7 +17147,7 @@
         <v>4.6506242492995673</v>
       </c>
       <c r="S30" s="129"/>
-      <c r="T30" s="173" t="s">
+      <c r="T30" s="174" t="s">
         <v>139</v>
       </c>
       <c r="U30" s="107">
@@ -17033,8 +17233,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:43">
-      <c r="A31" s="173"/>
+    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A31" s="174"/>
       <c r="B31" s="74">
         <f t="shared" ref="B31:B48" si="19">$B5</f>
         <v>650</v>
@@ -17104,7 +17304,7 @@
         <v>4.6506242492995673</v>
       </c>
       <c r="S31" s="129"/>
-      <c r="T31" s="173"/>
+      <c r="T31" s="174"/>
       <c r="U31" s="111">
         <v>650</v>
       </c>
@@ -17173,8 +17373,8 @@
         <v>8.384546476311888</v>
       </c>
     </row>
-    <row r="32" spans="1:43">
-      <c r="A32" s="173"/>
+    <row r="32" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A32" s="174"/>
       <c r="B32" s="74">
         <f t="shared" si="19"/>
         <v>800</v>
@@ -17244,7 +17444,7 @@
         <v>4.6704160099120591</v>
       </c>
       <c r="S32" s="129"/>
-      <c r="T32" s="173"/>
+      <c r="T32" s="174"/>
       <c r="U32" s="111">
         <v>800</v>
       </c>
@@ -17313,8 +17513,8 @@
         <v>8.384546476311888</v>
       </c>
     </row>
-    <row r="33" spans="1:37">
-      <c r="A33" s="173"/>
+    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A33" s="174"/>
       <c r="B33" s="74">
         <f t="shared" si="19"/>
         <v>1000</v>
@@ -17384,7 +17584,7 @@
         <v>4.6660032822574893</v>
       </c>
       <c r="S33" s="129"/>
-      <c r="T33" s="173"/>
+      <c r="T33" s="174"/>
       <c r="U33" s="111">
         <v>1000</v>
       </c>
@@ -17453,8 +17653,8 @@
         <v>8.384546476311888</v>
       </c>
     </row>
-    <row r="34" spans="1:37">
-      <c r="A34" s="173"/>
+    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A34" s="174"/>
       <c r="B34" s="74">
         <f t="shared" si="19"/>
         <v>1200</v>
@@ -17524,7 +17724,7 @@
         <v>4.5965170099601229</v>
       </c>
       <c r="S34" s="129"/>
-      <c r="T34" s="173"/>
+      <c r="T34" s="174"/>
       <c r="U34" s="111">
         <v>1200</v>
       </c>
@@ -17593,8 +17793,8 @@
         <v>8.384546476311888</v>
       </c>
     </row>
-    <row r="35" spans="1:37">
-      <c r="A35" s="173"/>
+    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A35" s="174"/>
       <c r="B35" s="74">
         <f t="shared" si="19"/>
         <v>1400</v>
@@ -17664,7 +17864,7 @@
         <v>4.4235917835667031</v>
       </c>
       <c r="S35" s="129"/>
-      <c r="T35" s="173"/>
+      <c r="T35" s="174"/>
       <c r="U35" s="111">
         <v>1400</v>
       </c>
@@ -17733,8 +17933,8 @@
         <v>8.4853915415781547</v>
       </c>
     </row>
-    <row r="36" spans="1:37">
-      <c r="A36" s="173"/>
+    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A36" s="174"/>
       <c r="B36" s="74">
         <f t="shared" si="19"/>
         <v>1550</v>
@@ -17804,7 +18004,7 @@
         <v>4.3862668647930958</v>
       </c>
       <c r="S36" s="129"/>
-      <c r="T36" s="173"/>
+      <c r="T36" s="174"/>
       <c r="U36" s="111">
         <v>1550</v>
       </c>
@@ -17873,8 +18073,8 @@
         <v>8.4274708078460154</v>
       </c>
     </row>
-    <row r="37" spans="1:37">
-      <c r="A37" s="173"/>
+    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A37" s="174"/>
       <c r="B37" s="74">
         <f t="shared" si="19"/>
         <v>1700</v>
@@ -17944,7 +18144,7 @@
         <v>4.357241798849568</v>
       </c>
       <c r="S37" s="129"/>
-      <c r="T37" s="173"/>
+      <c r="T37" s="174"/>
       <c r="U37" s="111">
         <v>1700</v>
       </c>
@@ -18013,8 +18213,8 @@
         <v>8.2860702549650753</v>
       </c>
     </row>
-    <row r="38" spans="1:37">
-      <c r="A38" s="173"/>
+    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A38" s="174"/>
       <c r="B38" s="74">
         <f t="shared" si="19"/>
         <v>1800</v>
@@ -18084,7 +18284,7 @@
         <v>4.3862668647930958</v>
       </c>
       <c r="S38" s="129"/>
-      <c r="T38" s="173"/>
+      <c r="T38" s="174"/>
       <c r="U38" s="111">
         <v>1800</v>
       </c>
@@ -18153,8 +18353,8 @@
         <v>7.9910969220289152</v>
       </c>
     </row>
-    <row r="39" spans="1:37">
-      <c r="A39" s="173"/>
+    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A39" s="174"/>
       <c r="B39" s="74">
         <f t="shared" si="19"/>
         <v>2000</v>
@@ -18224,7 +18424,7 @@
         <v>4.3862668647930958</v>
       </c>
       <c r="S39" s="129"/>
-      <c r="T39" s="173"/>
+      <c r="T39" s="174"/>
       <c r="U39" s="111">
         <v>2000</v>
       </c>
@@ -18293,8 +18493,8 @@
         <v>8.0431561604032922</v>
       </c>
     </row>
-    <row r="40" spans="1:37">
-      <c r="A40" s="173"/>
+    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A40" s="174"/>
       <c r="B40" s="74">
         <f t="shared" si="19"/>
         <v>2200</v>
@@ -18364,7 +18564,7 @@
         <v>4.3765489722677007</v>
       </c>
       <c r="S40" s="129"/>
-      <c r="T40" s="173"/>
+      <c r="T40" s="174"/>
       <c r="U40" s="111">
         <v>2200</v>
       </c>
@@ -18433,8 +18633,8 @@
         <v>7.7103791612385288</v>
       </c>
     </row>
-    <row r="41" spans="1:37">
-      <c r="A41" s="173"/>
+    <row r="41" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A41" s="174"/>
       <c r="B41" s="74">
         <f t="shared" si="19"/>
         <v>2400</v>
@@ -18504,7 +18704,7 @@
         <v>4.3823745508174383</v>
       </c>
       <c r="S41" s="129"/>
-      <c r="T41" s="173"/>
+      <c r="T41" s="174"/>
       <c r="U41" s="111">
         <v>2400</v>
       </c>
@@ -18573,8 +18773,8 @@
         <v>7.522464365334236</v>
       </c>
     </row>
-    <row r="42" spans="1:37">
-      <c r="A42" s="173"/>
+    <row r="42" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A42" s="174"/>
       <c r="B42" s="74">
         <f t="shared" si="19"/>
         <v>2600</v>
@@ -18644,7 +18844,7 @@
         <v>4.4295433567302318</v>
       </c>
       <c r="S42" s="129"/>
-      <c r="T42" s="173"/>
+      <c r="T42" s="174"/>
       <c r="U42" s="111">
         <v>2600</v>
       </c>
@@ -18713,8 +18913,8 @@
         <v>7.5396913534125041</v>
       </c>
     </row>
-    <row r="43" spans="1:37">
-      <c r="A43" s="173"/>
+    <row r="43" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A43" s="174"/>
       <c r="B43" s="74">
         <f t="shared" si="19"/>
         <v>2800</v>
@@ -18784,7 +18984,7 @@
         <v>4.139909347004985</v>
       </c>
       <c r="S43" s="129"/>
-      <c r="T43" s="173"/>
+      <c r="T43" s="174"/>
       <c r="U43" s="111">
         <v>2800</v>
       </c>
@@ -18853,8 +19053,8 @@
         <v>7.5396913534125041</v>
       </c>
     </row>
-    <row r="44" spans="1:37">
-      <c r="A44" s="173"/>
+    <row r="44" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A44" s="174"/>
       <c r="B44" s="74">
         <f t="shared" si="19"/>
         <v>2900</v>
@@ -18924,7 +19124,7 @@
         <v>4.1416453091752325</v>
       </c>
       <c r="S44" s="129"/>
-      <c r="T44" s="173"/>
+      <c r="T44" s="174"/>
       <c r="U44" s="111">
         <v>2900</v>
       </c>
@@ -18993,8 +19193,8 @@
         <v>7.5396913534125041</v>
       </c>
     </row>
-    <row r="45" spans="1:37">
-      <c r="A45" s="173"/>
+    <row r="45" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A45" s="174"/>
       <c r="B45" s="74">
         <f t="shared" si="19"/>
         <v>3000</v>
@@ -19064,7 +19264,7 @@
         <v>4.1468619418496857</v>
       </c>
       <c r="S45" s="129"/>
-      <c r="T45" s="173"/>
+      <c r="T45" s="174"/>
       <c r="U45" s="111">
         <v>3000</v>
       </c>
@@ -19133,8 +19333,8 @@
         <v>7.7103791612385288</v>
       </c>
     </row>
-    <row r="46" spans="1:37">
-      <c r="A46" s="173"/>
+    <row r="46" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A46" s="174"/>
       <c r="B46" s="74">
         <f t="shared" si="19"/>
         <v>3200</v>
@@ -19204,7 +19404,7 @@
         <v>4.2467089965984472</v>
       </c>
       <c r="S46" s="129"/>
-      <c r="T46" s="173"/>
+      <c r="T46" s="174"/>
       <c r="U46" s="111">
         <v>3200</v>
       </c>
@@ -19273,8 +19473,8 @@
         <v>8.1830950395136686</v>
       </c>
     </row>
-    <row r="47" spans="1:37">
-      <c r="A47" s="173"/>
+    <row r="47" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A47" s="174"/>
       <c r="B47" s="74">
         <f t="shared" si="19"/>
         <v>3300</v>
@@ -19344,7 +19544,7 @@
         <v>4.7927968555064169</v>
       </c>
       <c r="S47" s="129"/>
-      <c r="T47" s="173"/>
+      <c r="T47" s="174"/>
       <c r="U47" s="111">
         <v>3300</v>
       </c>
@@ -19413,7 +19613,7 @@
         <v>8.2860702549650753</v>
       </c>
     </row>
-    <row r="48" spans="1:37" ht="15.75" thickBot="1">
+    <row r="48" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="175"/>
       <c r="B48" s="89">
         <f t="shared" si="19"/>
@@ -19556,6 +19756,14 @@
   </sheetData>
   <sheetProtection password="CC3D" sheet="1" objects="1" scenarios="1" formatColumns="0"/>
   <mergeCells count="16">
+    <mergeCell ref="A30:A48"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="C2:R2"/>
+    <mergeCell ref="A4:A22"/>
+    <mergeCell ref="T28:U29"/>
+    <mergeCell ref="T30:T48"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A27:AK27"/>
     <mergeCell ref="A1:AK1"/>
     <mergeCell ref="AN28:AQ28"/>
     <mergeCell ref="T2:U3"/>
@@ -19564,21 +19772,13 @@
     <mergeCell ref="A28:B29"/>
     <mergeCell ref="C28:R28"/>
     <mergeCell ref="V28:AK28"/>
-    <mergeCell ref="A30:A48"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="C2:R2"/>
-    <mergeCell ref="A4:A22"/>
-    <mergeCell ref="T28:U29"/>
-    <mergeCell ref="T30:T48"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A27:AK27"/>
   </mergeCells>
   <conditionalFormatting sqref="C30:R48">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -19588,33 +19788,40 @@
   <conditionalFormatting sqref="V30:AK48">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Gear" prompt="Select the gear to view." sqref="A24:B24">
-      <formula1>Gear!G4:Z4</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Gear" prompt="Select the gear to view.">
+          <x14:formula1>
+            <xm:f>Gear!G4:Z4</xm:f>
+          </x14:formula1>
+          <xm:sqref>A24:B24</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" style="56" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" style="56" bestFit="1" customWidth="1"/>
@@ -19640,8 +19847,8 @@
     <col min="25" max="16384" width="8.85546875" style="56"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1"/>
-    <row r="2" spans="1:13" ht="15.75" thickBot="1">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>73</v>
       </c>
@@ -19656,7 +19863,7 @@
       <c r="L2" s="33"/>
       <c r="M2" s="33"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="34"/>
       <c r="B3" s="35" t="s">
         <v>58</v>
@@ -19692,7 +19899,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
         <v>60</v>
       </c>
@@ -19730,7 +19937,7 @@
         <v>6.09</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
         <v>61</v>
       </c>
@@ -19768,7 +19975,7 @@
         <v>6.55</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
         <v>62</v>
       </c>
@@ -19806,7 +20013,7 @@
         <v>3.58</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
         <v>63</v>
       </c>
@@ -19844,7 +20051,7 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
         <v>64</v>
       </c>
@@ -19882,7 +20089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
         <v>65</v>
       </c>
@@ -19916,7 +20123,7 @@
       <c r="K9" s="43"/>
       <c r="L9" s="62"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
         <v>66</v>
       </c>
@@ -19940,7 +20147,7 @@
       <c r="K10" s="40"/>
       <c r="L10" s="61"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
         <v>67</v>
       </c>
@@ -19956,7 +20163,7 @@
       <c r="K11" s="42"/>
       <c r="L11" s="45"/>
     </row>
-    <row r="12" spans="1:13" ht="15.75" thickBot="1">
+    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="48" t="s">
         <v>68</v>
       </c>
@@ -19972,8 +20179,8 @@
       <c r="K12" s="49"/>
       <c r="L12" s="63"/>
     </row>
-    <row r="13" spans="1:13" ht="15.75" thickBot="1"/>
-    <row r="14" spans="1:13" ht="15.75" thickBot="1">
+    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="32" t="s">
         <v>74</v>
       </c>
@@ -19988,7 +20195,7 @@
       <c r="L14" s="33"/>
       <c r="M14" s="33"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="34"/>
       <c r="B15" s="35" t="s">
         <v>85</v>
@@ -20024,7 +20231,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
         <v>60</v>
       </c>
@@ -20062,7 +20269,7 @@
         <v>2.0699999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="38" t="s">
         <v>61</v>
       </c>
@@ -20100,7 +20307,7 @@
         <v>2.48</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
         <v>62</v>
       </c>
@@ -20138,7 +20345,7 @@
         <v>1.48</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="38" t="s">
         <v>63</v>
       </c>
@@ -20176,7 +20383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
         <v>64</v>
       </c>
@@ -20212,7 +20419,7 @@
       </c>
       <c r="L20" s="41"/>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="38" t="s">
         <v>65</v>
       </c>
@@ -20240,7 +20447,7 @@
       <c r="K21" s="42"/>
       <c r="L21" s="47"/>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="38" t="s">
         <v>66</v>
       </c>
@@ -20266,7 +20473,7 @@
       <c r="K22" s="40"/>
       <c r="L22" s="41"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="38" t="s">
         <v>67</v>
       </c>
@@ -20284,7 +20491,7 @@
       <c r="K23" s="42"/>
       <c r="L23" s="45"/>
     </row>
-    <row r="24" spans="1:12" ht="15.75" thickBot="1">
+    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="48" t="s">
         <v>68</v>
       </c>
@@ -20302,13 +20509,13 @@
       <c r="K24" s="49"/>
       <c r="L24" s="50"/>
     </row>
-    <row r="25" spans="1:12" ht="15.75" thickBot="1"/>
-    <row r="26" spans="1:12" ht="15.75" thickBot="1">
+    <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="51" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="34"/>
       <c r="B27" s="35" t="s">
         <v>97</v>
@@ -20335,7 +20542,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15.75" thickBot="1">
+    <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="48" t="s">
         <v>104</v>
       </c>
@@ -20364,21 +20571,21 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="33" spans="2:4">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="186" t="s">
         <v>105</v>
       </c>
       <c r="C33" s="186"/>
       <c r="D33" s="186"/>
     </row>
-    <row r="34" spans="2:4">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="187" t="s">
         <v>106</v>
       </c>
       <c r="C34" s="187"/>
       <c r="D34" s="187"/>
     </row>
-    <row r="36" spans="2:4">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="57"/>
     </row>
   </sheetData>

</xml_diff>